<commit_message>
Jeez this is a lot of models to analyze
</commit_message>
<xml_diff>
--- a/NEW/statistical_analysis/Networks Compared.xlsx
+++ b/NEW/statistical_analysis/Networks Compared.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerhard\Documents\MSc-thesis\NEW\statistical_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F85312A-7F8B-4BD5-BF2D-1083F9D17873}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF94D25-5BC2-4C2B-B95B-FF302EF9DF90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="-120" windowWidth="27300" windowHeight="16440" activeTab="1" xr2:uid="{42FDFE43-F33F-4893-BA97-B5C32084F215}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="CNN (Conv2D)" sheetId="2" r:id="rId2"/>
     <sheet name="CNN (Conv1D)" sheetId="3" r:id="rId3"/>
     <sheet name="LSTM" sheetId="4" r:id="rId4"/>
+    <sheet name="XGBoost" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="55">
   <si>
     <t>Model Number</t>
   </si>
@@ -167,12 +168,45 @@
   <si>
     <t>All data, Scaled as follows: x=x-mean(x)/sd(x)</t>
   </si>
+  <si>
+    <t>M11</t>
+  </si>
+  <si>
+    <t>Full Dataset, All electron and twice that number of pions, 3 columns sequentially summed, scaled as follows x=x-mean(x)/sd(x)</t>
+  </si>
+  <si>
+    <t>Class Weights Used During Training</t>
+  </si>
+  <si>
+    <t>Full Dataset, All electron and twice that number of pions, features = 3 columns sequentially summed, and 24 timebin sums, columns scaled as follows x=x-mean(x)/sd(x)</t>
+  </si>
+  <si>
+    <t>All pions and an equal amount of electrons, Scaled as follows: x=x-mean(x)/sd(x)</t>
+  </si>
+  <si>
+    <t>M12</t>
+  </si>
+  <si>
+    <t>Model name</t>
+  </si>
+  <si>
+    <t>Number of Estimators</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Binary:Logistic</t>
+  </si>
+  <si>
+    <t>Column sums, all electrons and an equal number of pions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +216,20 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -204,13 +252,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -523,11 +575,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32EF017-127E-4272-A45C-8B2FC1D130CC}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:O7"/>
+      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,16 +591,17 @@
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="154.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,40 +627,346 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
-        <v>32</v>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>32</v>
+      </c>
+      <c r="H2">
+        <v>0.01</v>
+      </c>
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="L2">
+        <v>0.65</v>
+      </c>
+      <c r="M2">
+        <v>0.6</v>
+      </c>
+      <c r="N2">
+        <v>0.9</v>
+      </c>
+      <c r="O2">
+        <v>0.9</v>
+      </c>
+      <c r="P2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>32</v>
+      </c>
+      <c r="H3">
+        <v>0.01</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>0.65</v>
+      </c>
+      <c r="M3">
+        <v>0.6</v>
+      </c>
+      <c r="N3">
+        <v>0.9</v>
+      </c>
+      <c r="O3">
+        <v>0.9</v>
+      </c>
+      <c r="P3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>32</v>
+      </c>
+      <c r="H4">
+        <v>0.01</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>0.74</v>
+      </c>
+      <c r="M4">
+        <v>0.745</v>
+      </c>
+      <c r="N4">
+        <v>0.9</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="P4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>32</v>
+      </c>
+      <c r="H5">
+        <v>0.01</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+      <c r="L5">
+        <v>0.74</v>
+      </c>
+      <c r="M5">
+        <v>0.745</v>
+      </c>
+      <c r="N5">
+        <v>0.9</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="P5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>128</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>32</v>
+      </c>
+      <c r="H6">
+        <v>0.01</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>50</v>
+      </c>
+      <c r="L6">
+        <v>0.79</v>
+      </c>
+      <c r="M6">
+        <v>0.79</v>
+      </c>
+      <c r="N6">
+        <v>0.9</v>
+      </c>
+      <c r="O6">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="P6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>128</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>32</v>
+      </c>
+      <c r="H7">
+        <v>0.01</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>50</v>
+      </c>
+      <c r="L7">
+        <v>0.79</v>
+      </c>
+      <c r="M7">
+        <v>0.79</v>
+      </c>
+      <c r="N7">
+        <v>0.9</v>
+      </c>
+      <c r="O7">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="P7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>32</v>
+      </c>
+      <c r="H8">
+        <v>0.01</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>50</v>
+      </c>
+      <c r="L8">
+        <v>0.79</v>
+      </c>
+      <c r="M8">
+        <v>0.79</v>
+      </c>
+      <c r="N8">
+        <v>0.9</v>
+      </c>
+      <c r="O8">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="P8" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D847C349-F495-423A-9F1C-FAD29C38B92F}">
-  <dimension ref="A1:S95"/>
+  <dimension ref="A1:S129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S97" sqref="S97"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S112" sqref="S112:S129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +987,7 @@
     <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="74.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -4175,28 +4534,28 @@
         <v>5</v>
       </c>
       <c r="K89">
-        <v>100000</v>
+        <v>32</v>
       </c>
       <c r="L89">
         <v>0.01</v>
       </c>
       <c r="N89">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="O89">
-        <v>90.6</v>
+        <v>0.91249999999999998</v>
       </c>
       <c r="P89">
-        <v>90.5</v>
+        <v>0.90749999999999997</v>
       </c>
       <c r="Q89">
-        <v>0.89700000000000002</v>
+        <v>0.753</v>
       </c>
       <c r="R89">
-        <v>0.75900000000000001</v>
+        <v>0.54</v>
       </c>
       <c r="S89" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
@@ -4215,6 +4574,12 @@
       <c r="E90" t="s">
         <v>20</v>
       </c>
+      <c r="F90" t="b">
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <v>0.25</v>
+      </c>
       <c r="I90" t="s">
         <v>4</v>
       </c>
@@ -4222,28 +4587,28 @@
         <v>5</v>
       </c>
       <c r="K90">
-        <v>100000</v>
+        <v>32</v>
       </c>
       <c r="L90">
         <v>0.01</v>
       </c>
       <c r="N90">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="O90">
-        <v>90.6</v>
+        <v>0.91249999999999998</v>
       </c>
       <c r="P90">
-        <v>90.5</v>
+        <v>0.90749999999999997</v>
       </c>
       <c r="Q90">
-        <v>0.89700000000000002</v>
+        <v>0.753</v>
       </c>
       <c r="R90">
-        <v>0.75900000000000001</v>
+        <v>0.54</v>
       </c>
       <c r="S90" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
@@ -4253,20 +4618,11 @@
       <c r="B91">
         <v>3</v>
       </c>
-      <c r="C91" t="b">
-        <v>1</v>
-      </c>
-      <c r="D91">
-        <v>64</v>
-      </c>
-      <c r="E91" t="s">
-        <v>30</v>
-      </c>
-      <c r="F91" t="b">
-        <v>1</v>
-      </c>
       <c r="G91">
-        <v>0.25</v>
+        <v>0.5</v>
+      </c>
+      <c r="H91">
+        <v>128</v>
       </c>
       <c r="I91" t="s">
         <v>4</v>
@@ -4275,28 +4631,28 @@
         <v>5</v>
       </c>
       <c r="K91">
-        <v>100000</v>
+        <v>32</v>
       </c>
       <c r="L91">
         <v>0.01</v>
       </c>
       <c r="N91">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="O91">
-        <v>90.6</v>
+        <v>0.91249999999999998</v>
       </c>
       <c r="P91">
-        <v>90.5</v>
+        <v>0.90749999999999997</v>
       </c>
       <c r="Q91">
-        <v>0.89700000000000002</v>
+        <v>0.753</v>
       </c>
       <c r="R91">
-        <v>0.75900000000000001</v>
+        <v>0.54</v>
       </c>
       <c r="S91" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
@@ -4306,41 +4662,38 @@
       <c r="B92">
         <v>4</v>
       </c>
-      <c r="G92">
-        <v>0.5</v>
-      </c>
       <c r="H92">
-        <v>256</v>
+        <v>2</v>
       </c>
       <c r="I92" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="J92" t="s">
         <v>5</v>
       </c>
       <c r="K92">
-        <v>100000</v>
+        <v>32</v>
       </c>
       <c r="L92">
         <v>0.01</v>
       </c>
       <c r="N92">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="O92">
-        <v>90.6</v>
+        <v>0.91249999999999998</v>
       </c>
       <c r="P92">
-        <v>90.5</v>
+        <v>0.90749999999999997</v>
       </c>
       <c r="Q92">
-        <v>0.89700000000000002</v>
+        <v>0.753</v>
       </c>
       <c r="R92">
-        <v>0.75900000000000001</v>
+        <v>0.54</v>
       </c>
       <c r="S92" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
@@ -4348,13 +4701,16 @@
         <v>42</v>
       </c>
       <c r="B93">
-        <v>5</v>
-      </c>
-      <c r="G93">
-        <v>0.5</v>
-      </c>
-      <c r="H93">
-        <v>128</v>
+        <v>1</v>
+      </c>
+      <c r="C93" t="b">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>32</v>
+      </c>
+      <c r="E93" t="s">
+        <v>20</v>
       </c>
       <c r="I93" t="s">
         <v>4</v>
@@ -4372,10 +4728,10 @@
         <v>40</v>
       </c>
       <c r="O93">
-        <v>90.6</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="P93">
-        <v>90.5</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="Q93">
         <v>0.89700000000000002</v>
@@ -4392,13 +4748,16 @@
         <v>42</v>
       </c>
       <c r="B94">
-        <v>6</v>
-      </c>
-      <c r="G94">
-        <v>0.5</v>
-      </c>
-      <c r="H94">
-        <v>128</v>
+        <v>2</v>
+      </c>
+      <c r="C94" t="b">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>64</v>
+      </c>
+      <c r="E94" t="s">
+        <v>20</v>
       </c>
       <c r="I94" t="s">
         <v>4</v>
@@ -4416,10 +4775,10 @@
         <v>40</v>
       </c>
       <c r="O94">
-        <v>90.6</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="P94">
-        <v>90.5</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="Q94">
         <v>0.89700000000000002</v>
@@ -4436,13 +4795,25 @@
         <v>42</v>
       </c>
       <c r="B95">
-        <v>7</v>
-      </c>
-      <c r="H95">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C95" t="b">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>64</v>
+      </c>
+      <c r="E95" t="s">
+        <v>30</v>
+      </c>
+      <c r="F95" t="b">
+        <v>1</v>
+      </c>
+      <c r="G95">
+        <v>0.25</v>
       </c>
       <c r="I95" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="J95" t="s">
         <v>5</v>
@@ -4457,10 +4828,10 @@
         <v>40</v>
       </c>
       <c r="O95">
-        <v>90.6</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="P95">
-        <v>90.5</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="Q95">
         <v>0.89700000000000002</v>
@@ -4470,6 +4841,1439 @@
       </c>
       <c r="S95" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>42</v>
+      </c>
+      <c r="B96">
+        <v>4</v>
+      </c>
+      <c r="G96">
+        <v>0.5</v>
+      </c>
+      <c r="H96">
+        <v>256</v>
+      </c>
+      <c r="I96" t="s">
+        <v>4</v>
+      </c>
+      <c r="J96" t="s">
+        <v>5</v>
+      </c>
+      <c r="K96">
+        <v>100000</v>
+      </c>
+      <c r="L96">
+        <v>0.01</v>
+      </c>
+      <c r="N96">
+        <v>40</v>
+      </c>
+      <c r="O96">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="P96">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="Q96">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="R96">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="S96" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>42</v>
+      </c>
+      <c r="B97">
+        <v>5</v>
+      </c>
+      <c r="G97">
+        <v>0.5</v>
+      </c>
+      <c r="H97">
+        <v>128</v>
+      </c>
+      <c r="I97" t="s">
+        <v>4</v>
+      </c>
+      <c r="J97" t="s">
+        <v>5</v>
+      </c>
+      <c r="K97">
+        <v>100000</v>
+      </c>
+      <c r="L97">
+        <v>0.01</v>
+      </c>
+      <c r="N97">
+        <v>40</v>
+      </c>
+      <c r="O97">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="P97">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="Q97">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="R97">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="S97" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>42</v>
+      </c>
+      <c r="B98">
+        <v>6</v>
+      </c>
+      <c r="G98">
+        <v>0.5</v>
+      </c>
+      <c r="H98">
+        <v>128</v>
+      </c>
+      <c r="I98" t="s">
+        <v>4</v>
+      </c>
+      <c r="J98" t="s">
+        <v>5</v>
+      </c>
+      <c r="K98">
+        <v>100000</v>
+      </c>
+      <c r="L98">
+        <v>0.01</v>
+      </c>
+      <c r="N98">
+        <v>40</v>
+      </c>
+      <c r="O98">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="P98">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="Q98">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="R98">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="S98" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>42</v>
+      </c>
+      <c r="B99">
+        <v>7</v>
+      </c>
+      <c r="H99">
+        <v>2</v>
+      </c>
+      <c r="I99" t="s">
+        <v>26</v>
+      </c>
+      <c r="J99" t="s">
+        <v>5</v>
+      </c>
+      <c r="K99">
+        <v>100000</v>
+      </c>
+      <c r="L99">
+        <v>0.01</v>
+      </c>
+      <c r="N99">
+        <v>40</v>
+      </c>
+      <c r="O99">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="P99">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="Q99">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="R99">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="S99" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>44</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100" t="b">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>32</v>
+      </c>
+      <c r="E100" t="s">
+        <v>19</v>
+      </c>
+      <c r="I100" t="s">
+        <v>33</v>
+      </c>
+      <c r="J100" t="s">
+        <v>5</v>
+      </c>
+      <c r="K100">
+        <v>32</v>
+      </c>
+      <c r="L100">
+        <v>0.01</v>
+      </c>
+      <c r="N100">
+        <v>100</v>
+      </c>
+      <c r="O100">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P100">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q100">
+        <v>0.9</v>
+      </c>
+      <c r="R100">
+        <v>0.89</v>
+      </c>
+      <c r="S100" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>44</v>
+      </c>
+      <c r="B101">
+        <v>2</v>
+      </c>
+      <c r="C101" t="b">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>64</v>
+      </c>
+      <c r="E101" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" t="b">
+        <v>1</v>
+      </c>
+      <c r="I101" t="s">
+        <v>4</v>
+      </c>
+      <c r="J101" t="s">
+        <v>5</v>
+      </c>
+      <c r="K101">
+        <v>32</v>
+      </c>
+      <c r="L101">
+        <v>0.01</v>
+      </c>
+      <c r="N101">
+        <v>100</v>
+      </c>
+      <c r="O101">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P101">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q101">
+        <v>0.9</v>
+      </c>
+      <c r="R101">
+        <v>0.89</v>
+      </c>
+      <c r="S101" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>44</v>
+      </c>
+      <c r="B102">
+        <v>3</v>
+      </c>
+      <c r="H102">
+        <v>256</v>
+      </c>
+      <c r="I102" t="s">
+        <v>4</v>
+      </c>
+      <c r="J102" t="s">
+        <v>5</v>
+      </c>
+      <c r="K102">
+        <v>32</v>
+      </c>
+      <c r="L102">
+        <v>0.01</v>
+      </c>
+      <c r="N102">
+        <v>100</v>
+      </c>
+      <c r="O102">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P102">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q102">
+        <v>0.9</v>
+      </c>
+      <c r="R102">
+        <v>0.89</v>
+      </c>
+      <c r="S102" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>44</v>
+      </c>
+      <c r="B103">
+        <v>4</v>
+      </c>
+      <c r="H103">
+        <v>256</v>
+      </c>
+      <c r="I103" t="s">
+        <v>4</v>
+      </c>
+      <c r="J103" t="s">
+        <v>5</v>
+      </c>
+      <c r="K103">
+        <v>32</v>
+      </c>
+      <c r="L103">
+        <v>0.01</v>
+      </c>
+      <c r="N103">
+        <v>100</v>
+      </c>
+      <c r="O103">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P103">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q103">
+        <v>0.9</v>
+      </c>
+      <c r="R103">
+        <v>0.89</v>
+      </c>
+      <c r="S103" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>44</v>
+      </c>
+      <c r="B104">
+        <v>5</v>
+      </c>
+      <c r="H104">
+        <v>256</v>
+      </c>
+      <c r="I104" t="s">
+        <v>4</v>
+      </c>
+      <c r="J104" t="s">
+        <v>5</v>
+      </c>
+      <c r="K104">
+        <v>32</v>
+      </c>
+      <c r="L104">
+        <v>0.01</v>
+      </c>
+      <c r="N104">
+        <v>100</v>
+      </c>
+      <c r="O104">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P104">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q104">
+        <v>0.9</v>
+      </c>
+      <c r="R104">
+        <v>0.89</v>
+      </c>
+      <c r="S104" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>44</v>
+      </c>
+      <c r="B105">
+        <v>6</v>
+      </c>
+      <c r="H105">
+        <v>256</v>
+      </c>
+      <c r="I105" t="s">
+        <v>4</v>
+      </c>
+      <c r="J105" t="s">
+        <v>5</v>
+      </c>
+      <c r="K105">
+        <v>32</v>
+      </c>
+      <c r="L105">
+        <v>0.01</v>
+      </c>
+      <c r="N105">
+        <v>100</v>
+      </c>
+      <c r="O105">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P105">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q105">
+        <v>0.9</v>
+      </c>
+      <c r="R105">
+        <v>0.89</v>
+      </c>
+      <c r="S105" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>44</v>
+      </c>
+      <c r="B106">
+        <v>7</v>
+      </c>
+      <c r="H106">
+        <v>256</v>
+      </c>
+      <c r="I106" t="s">
+        <v>4</v>
+      </c>
+      <c r="J106" t="s">
+        <v>5</v>
+      </c>
+      <c r="K106">
+        <v>32</v>
+      </c>
+      <c r="L106">
+        <v>0.01</v>
+      </c>
+      <c r="N106">
+        <v>100</v>
+      </c>
+      <c r="O106">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P106">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q106">
+        <v>0.9</v>
+      </c>
+      <c r="R106">
+        <v>0.89</v>
+      </c>
+      <c r="S106" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>44</v>
+      </c>
+      <c r="B107">
+        <v>8</v>
+      </c>
+      <c r="H107">
+        <v>256</v>
+      </c>
+      <c r="I107" t="s">
+        <v>4</v>
+      </c>
+      <c r="J107" t="s">
+        <v>5</v>
+      </c>
+      <c r="K107">
+        <v>32</v>
+      </c>
+      <c r="L107">
+        <v>0.01</v>
+      </c>
+      <c r="N107">
+        <v>100</v>
+      </c>
+      <c r="O107">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P107">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q107">
+        <v>0.9</v>
+      </c>
+      <c r="R107">
+        <v>0.89</v>
+      </c>
+      <c r="S107" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>44</v>
+      </c>
+      <c r="B108">
+        <v>9</v>
+      </c>
+      <c r="H108">
+        <v>256</v>
+      </c>
+      <c r="I108" t="s">
+        <v>4</v>
+      </c>
+      <c r="J108" t="s">
+        <v>5</v>
+      </c>
+      <c r="K108">
+        <v>32</v>
+      </c>
+      <c r="L108">
+        <v>0.01</v>
+      </c>
+      <c r="N108">
+        <v>100</v>
+      </c>
+      <c r="O108">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P108">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q108">
+        <v>0.9</v>
+      </c>
+      <c r="R108">
+        <v>0.89</v>
+      </c>
+      <c r="S108" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>44</v>
+      </c>
+      <c r="B109">
+        <v>10</v>
+      </c>
+      <c r="H109">
+        <v>256</v>
+      </c>
+      <c r="I109" t="s">
+        <v>4</v>
+      </c>
+      <c r="J109" t="s">
+        <v>5</v>
+      </c>
+      <c r="K109">
+        <v>32</v>
+      </c>
+      <c r="L109">
+        <v>0.01</v>
+      </c>
+      <c r="N109">
+        <v>100</v>
+      </c>
+      <c r="O109">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P109">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q109">
+        <v>0.9</v>
+      </c>
+      <c r="R109">
+        <v>0.89</v>
+      </c>
+      <c r="S109" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>44</v>
+      </c>
+      <c r="B110">
+        <v>11</v>
+      </c>
+      <c r="H110">
+        <v>256</v>
+      </c>
+      <c r="I110" t="s">
+        <v>4</v>
+      </c>
+      <c r="J110" t="s">
+        <v>5</v>
+      </c>
+      <c r="K110">
+        <v>32</v>
+      </c>
+      <c r="L110">
+        <v>0.01</v>
+      </c>
+      <c r="N110">
+        <v>100</v>
+      </c>
+      <c r="O110">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P110">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q110">
+        <v>0.9</v>
+      </c>
+      <c r="R110">
+        <v>0.89</v>
+      </c>
+      <c r="S110" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>44</v>
+      </c>
+      <c r="B111">
+        <v>12</v>
+      </c>
+      <c r="H111">
+        <v>256</v>
+      </c>
+      <c r="I111" t="s">
+        <v>4</v>
+      </c>
+      <c r="J111" t="s">
+        <v>5</v>
+      </c>
+      <c r="K111">
+        <v>32</v>
+      </c>
+      <c r="L111">
+        <v>0.01</v>
+      </c>
+      <c r="N111">
+        <v>100</v>
+      </c>
+      <c r="O111">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P111">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q111">
+        <v>0.9</v>
+      </c>
+      <c r="R111">
+        <v>0.89</v>
+      </c>
+      <c r="S111" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>44</v>
+      </c>
+      <c r="B112">
+        <v>13</v>
+      </c>
+      <c r="H112">
+        <v>2</v>
+      </c>
+      <c r="I112" t="s">
+        <v>26</v>
+      </c>
+      <c r="J112" t="s">
+        <v>5</v>
+      </c>
+      <c r="K112">
+        <v>32</v>
+      </c>
+      <c r="L112">
+        <v>0.01</v>
+      </c>
+      <c r="N112">
+        <v>100</v>
+      </c>
+      <c r="O112">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P112">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q112">
+        <v>0.9</v>
+      </c>
+      <c r="R112">
+        <v>0.89</v>
+      </c>
+      <c r="S112" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>49</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+      <c r="C113" t="b">
+        <v>1</v>
+      </c>
+      <c r="D113">
+        <v>32</v>
+      </c>
+      <c r="E113" t="s">
+        <v>19</v>
+      </c>
+      <c r="I113" t="s">
+        <v>33</v>
+      </c>
+      <c r="J113" t="s">
+        <v>5</v>
+      </c>
+      <c r="K113">
+        <v>32</v>
+      </c>
+      <c r="L113">
+        <v>0.01</v>
+      </c>
+      <c r="N113">
+        <v>100</v>
+      </c>
+      <c r="O113">
+        <v>0.9</v>
+      </c>
+      <c r="P113">
+        <v>0.51</v>
+      </c>
+      <c r="Q113">
+        <v>0.9</v>
+      </c>
+      <c r="R113">
+        <v>0.9</v>
+      </c>
+      <c r="S113" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>49</v>
+      </c>
+      <c r="B114">
+        <v>2</v>
+      </c>
+      <c r="C114" t="b">
+        <v>1</v>
+      </c>
+      <c r="D114">
+        <v>64</v>
+      </c>
+      <c r="E114" t="s">
+        <v>19</v>
+      </c>
+      <c r="F114" t="b">
+        <v>1</v>
+      </c>
+      <c r="I114" t="s">
+        <v>33</v>
+      </c>
+      <c r="J114" t="s">
+        <v>5</v>
+      </c>
+      <c r="K114">
+        <v>32</v>
+      </c>
+      <c r="L114">
+        <v>0.01</v>
+      </c>
+      <c r="N114">
+        <v>100</v>
+      </c>
+      <c r="O114">
+        <v>0.9</v>
+      </c>
+      <c r="P114">
+        <v>0.51</v>
+      </c>
+      <c r="Q114">
+        <v>0.9</v>
+      </c>
+      <c r="R114">
+        <v>0.9</v>
+      </c>
+      <c r="S114" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>49</v>
+      </c>
+      <c r="B115">
+        <v>3</v>
+      </c>
+      <c r="H115">
+        <v>512</v>
+      </c>
+      <c r="I115" t="s">
+        <v>4</v>
+      </c>
+      <c r="J115" t="s">
+        <v>5</v>
+      </c>
+      <c r="K115">
+        <v>32</v>
+      </c>
+      <c r="L115">
+        <v>0.01</v>
+      </c>
+      <c r="N115">
+        <v>100</v>
+      </c>
+      <c r="O115">
+        <v>0.9</v>
+      </c>
+      <c r="P115">
+        <v>0.51</v>
+      </c>
+      <c r="Q115">
+        <v>0.9</v>
+      </c>
+      <c r="R115">
+        <v>0.9</v>
+      </c>
+      <c r="S115" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>49</v>
+      </c>
+      <c r="B116">
+        <v>4</v>
+      </c>
+      <c r="H116">
+        <v>512</v>
+      </c>
+      <c r="I116" t="s">
+        <v>4</v>
+      </c>
+      <c r="J116" t="s">
+        <v>5</v>
+      </c>
+      <c r="K116">
+        <v>32</v>
+      </c>
+      <c r="L116">
+        <v>0.01</v>
+      </c>
+      <c r="N116">
+        <v>100</v>
+      </c>
+      <c r="O116">
+        <v>0.9</v>
+      </c>
+      <c r="P116">
+        <v>0.51</v>
+      </c>
+      <c r="Q116">
+        <v>0.9</v>
+      </c>
+      <c r="R116">
+        <v>0.9</v>
+      </c>
+      <c r="S116" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>49</v>
+      </c>
+      <c r="B117">
+        <v>5</v>
+      </c>
+      <c r="H117">
+        <v>512</v>
+      </c>
+      <c r="I117" t="s">
+        <v>4</v>
+      </c>
+      <c r="J117" t="s">
+        <v>5</v>
+      </c>
+      <c r="K117">
+        <v>32</v>
+      </c>
+      <c r="L117">
+        <v>0.01</v>
+      </c>
+      <c r="N117">
+        <v>100</v>
+      </c>
+      <c r="O117">
+        <v>0.9</v>
+      </c>
+      <c r="P117">
+        <v>0.51</v>
+      </c>
+      <c r="Q117">
+        <v>0.9</v>
+      </c>
+      <c r="R117">
+        <v>0.9</v>
+      </c>
+      <c r="S117" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>49</v>
+      </c>
+      <c r="B118">
+        <v>6</v>
+      </c>
+      <c r="H118">
+        <v>512</v>
+      </c>
+      <c r="I118" t="s">
+        <v>4</v>
+      </c>
+      <c r="J118" t="s">
+        <v>5</v>
+      </c>
+      <c r="K118">
+        <v>32</v>
+      </c>
+      <c r="L118">
+        <v>0.01</v>
+      </c>
+      <c r="N118">
+        <v>100</v>
+      </c>
+      <c r="O118">
+        <v>0.9</v>
+      </c>
+      <c r="P118">
+        <v>0.51</v>
+      </c>
+      <c r="Q118">
+        <v>0.9</v>
+      </c>
+      <c r="R118">
+        <v>0.9</v>
+      </c>
+      <c r="S118" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>49</v>
+      </c>
+      <c r="B119">
+        <v>7</v>
+      </c>
+      <c r="H119">
+        <v>512</v>
+      </c>
+      <c r="I119" t="s">
+        <v>4</v>
+      </c>
+      <c r="J119" t="s">
+        <v>5</v>
+      </c>
+      <c r="K119">
+        <v>32</v>
+      </c>
+      <c r="L119">
+        <v>0.01</v>
+      </c>
+      <c r="N119">
+        <v>100</v>
+      </c>
+      <c r="O119">
+        <v>0.9</v>
+      </c>
+      <c r="P119">
+        <v>0.51</v>
+      </c>
+      <c r="Q119">
+        <v>0.9</v>
+      </c>
+      <c r="R119">
+        <v>0.9</v>
+      </c>
+      <c r="S119" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>49</v>
+      </c>
+      <c r="B120">
+        <v>8</v>
+      </c>
+      <c r="H120">
+        <v>512</v>
+      </c>
+      <c r="I120" t="s">
+        <v>4</v>
+      </c>
+      <c r="J120" t="s">
+        <v>5</v>
+      </c>
+      <c r="K120">
+        <v>32</v>
+      </c>
+      <c r="L120">
+        <v>0.01</v>
+      </c>
+      <c r="N120">
+        <v>100</v>
+      </c>
+      <c r="O120">
+        <v>0.9</v>
+      </c>
+      <c r="P120">
+        <v>0.51</v>
+      </c>
+      <c r="Q120">
+        <v>0.9</v>
+      </c>
+      <c r="R120">
+        <v>0.9</v>
+      </c>
+      <c r="S120" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>49</v>
+      </c>
+      <c r="B121">
+        <v>9</v>
+      </c>
+      <c r="H121">
+        <v>512</v>
+      </c>
+      <c r="I121" t="s">
+        <v>4</v>
+      </c>
+      <c r="J121" t="s">
+        <v>5</v>
+      </c>
+      <c r="K121">
+        <v>32</v>
+      </c>
+      <c r="L121">
+        <v>0.01</v>
+      </c>
+      <c r="N121">
+        <v>100</v>
+      </c>
+      <c r="O121">
+        <v>0.9</v>
+      </c>
+      <c r="P121">
+        <v>0.51</v>
+      </c>
+      <c r="Q121">
+        <v>0.9</v>
+      </c>
+      <c r="R121">
+        <v>0.9</v>
+      </c>
+      <c r="S121" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>49</v>
+      </c>
+      <c r="B122">
+        <v>10</v>
+      </c>
+      <c r="H122">
+        <v>512</v>
+      </c>
+      <c r="I122" t="s">
+        <v>4</v>
+      </c>
+      <c r="J122" t="s">
+        <v>5</v>
+      </c>
+      <c r="K122">
+        <v>32</v>
+      </c>
+      <c r="L122">
+        <v>0.01</v>
+      </c>
+      <c r="N122">
+        <v>100</v>
+      </c>
+      <c r="O122">
+        <v>0.9</v>
+      </c>
+      <c r="P122">
+        <v>0.51</v>
+      </c>
+      <c r="Q122">
+        <v>0.9</v>
+      </c>
+      <c r="R122">
+        <v>0.9</v>
+      </c>
+      <c r="S122" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>49</v>
+      </c>
+      <c r="B123">
+        <v>11</v>
+      </c>
+      <c r="H123">
+        <v>512</v>
+      </c>
+      <c r="I123" t="s">
+        <v>4</v>
+      </c>
+      <c r="J123" t="s">
+        <v>5</v>
+      </c>
+      <c r="K123">
+        <v>32</v>
+      </c>
+      <c r="L123">
+        <v>0.01</v>
+      </c>
+      <c r="N123">
+        <v>100</v>
+      </c>
+      <c r="O123">
+        <v>0.9</v>
+      </c>
+      <c r="P123">
+        <v>0.51</v>
+      </c>
+      <c r="Q123">
+        <v>0.9</v>
+      </c>
+      <c r="R123">
+        <v>0.9</v>
+      </c>
+      <c r="S123" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>49</v>
+      </c>
+      <c r="B124">
+        <v>12</v>
+      </c>
+      <c r="H124">
+        <v>512</v>
+      </c>
+      <c r="I124" t="s">
+        <v>4</v>
+      </c>
+      <c r="J124" t="s">
+        <v>5</v>
+      </c>
+      <c r="K124">
+        <v>32</v>
+      </c>
+      <c r="L124">
+        <v>0.01</v>
+      </c>
+      <c r="N124">
+        <v>100</v>
+      </c>
+      <c r="O124">
+        <v>0.9</v>
+      </c>
+      <c r="P124">
+        <v>0.51</v>
+      </c>
+      <c r="Q124">
+        <v>0.9</v>
+      </c>
+      <c r="R124">
+        <v>0.9</v>
+      </c>
+      <c r="S124" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>49</v>
+      </c>
+      <c r="B125">
+        <v>13</v>
+      </c>
+      <c r="H125">
+        <v>512</v>
+      </c>
+      <c r="I125" t="s">
+        <v>4</v>
+      </c>
+      <c r="J125" t="s">
+        <v>5</v>
+      </c>
+      <c r="K125">
+        <v>32</v>
+      </c>
+      <c r="L125">
+        <v>0.01</v>
+      </c>
+      <c r="N125">
+        <v>100</v>
+      </c>
+      <c r="O125">
+        <v>0.9</v>
+      </c>
+      <c r="P125">
+        <v>0.51</v>
+      </c>
+      <c r="Q125">
+        <v>0.9</v>
+      </c>
+      <c r="R125">
+        <v>0.9</v>
+      </c>
+      <c r="S125" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>49</v>
+      </c>
+      <c r="B126">
+        <v>14</v>
+      </c>
+      <c r="H126">
+        <v>512</v>
+      </c>
+      <c r="I126" t="s">
+        <v>4</v>
+      </c>
+      <c r="J126" t="s">
+        <v>5</v>
+      </c>
+      <c r="K126">
+        <v>32</v>
+      </c>
+      <c r="L126">
+        <v>0.01</v>
+      </c>
+      <c r="N126">
+        <v>100</v>
+      </c>
+      <c r="O126">
+        <v>0.9</v>
+      </c>
+      <c r="P126">
+        <v>0.51</v>
+      </c>
+      <c r="Q126">
+        <v>0.9</v>
+      </c>
+      <c r="R126">
+        <v>0.9</v>
+      </c>
+      <c r="S126" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>49</v>
+      </c>
+      <c r="B127">
+        <v>15</v>
+      </c>
+      <c r="H127">
+        <v>512</v>
+      </c>
+      <c r="I127" t="s">
+        <v>4</v>
+      </c>
+      <c r="J127" t="s">
+        <v>5</v>
+      </c>
+      <c r="K127">
+        <v>32</v>
+      </c>
+      <c r="L127">
+        <v>0.01</v>
+      </c>
+      <c r="N127">
+        <v>100</v>
+      </c>
+      <c r="O127">
+        <v>0.9</v>
+      </c>
+      <c r="P127">
+        <v>0.51</v>
+      </c>
+      <c r="Q127">
+        <v>0.9</v>
+      </c>
+      <c r="R127">
+        <v>0.9</v>
+      </c>
+      <c r="S127" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>49</v>
+      </c>
+      <c r="B128">
+        <v>16</v>
+      </c>
+      <c r="H128">
+        <v>512</v>
+      </c>
+      <c r="I128" t="s">
+        <v>4</v>
+      </c>
+      <c r="J128" t="s">
+        <v>5</v>
+      </c>
+      <c r="K128">
+        <v>32</v>
+      </c>
+      <c r="L128">
+        <v>0.01</v>
+      </c>
+      <c r="N128">
+        <v>100</v>
+      </c>
+      <c r="O128">
+        <v>0.9</v>
+      </c>
+      <c r="P128">
+        <v>0.51</v>
+      </c>
+      <c r="Q128">
+        <v>0.9</v>
+      </c>
+      <c r="R128">
+        <v>0.9</v>
+      </c>
+      <c r="S128" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>49</v>
+      </c>
+      <c r="B129">
+        <v>17</v>
+      </c>
+      <c r="H129">
+        <v>2</v>
+      </c>
+      <c r="I129" t="s">
+        <v>26</v>
+      </c>
+      <c r="J129" t="s">
+        <v>5</v>
+      </c>
+      <c r="K129">
+        <v>32</v>
+      </c>
+      <c r="L129">
+        <v>0.01</v>
+      </c>
+      <c r="N129">
+        <v>100</v>
+      </c>
+      <c r="O129">
+        <v>0.9</v>
+      </c>
+      <c r="P129">
+        <v>0.51</v>
+      </c>
+      <c r="Q129">
+        <v>0.9</v>
+      </c>
+      <c r="R129">
+        <v>0.9</v>
+      </c>
+      <c r="S129" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -4494,7 +6298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26382EEA-56AD-452C-9D78-7AC7571B137C}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
@@ -4936,4 +6740,67 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98088B90-BB92-4A82-86B2-658E03FA1477}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2">
+        <v>0.9</v>
+      </c>
+      <c r="E2">
+        <v>0.8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Still analyzing and comparing old models
</commit_message>
<xml_diff>
--- a/NEW/statistical_analysis/Networks Compared.xlsx
+++ b/NEW/statistical_analysis/Networks Compared.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerhard\Documents\MSc-thesis\NEW\statistical_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF94D25-5BC2-4C2B-B95B-FF302EF9DF90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823623B6-7A25-43BB-856C-1621BCA9122B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="-120" windowWidth="27300" windowHeight="16440" activeTab="1" xr2:uid="{42FDFE43-F33F-4893-BA97-B5C32084F215}"/>
+    <workbookView xWindow="-22212" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{42FDFE43-F33F-4893-BA97-B5C32084F215}"/>
   </bookViews>
   <sheets>
     <sheet name="Fully conected" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="58">
   <si>
     <t>Model Number</t>
   </si>
@@ -200,6 +200,15 @@
   </si>
   <si>
     <t>Column sums, all electrons and an equal number of pions</t>
+  </si>
+  <si>
+    <t>M13</t>
+  </si>
+  <si>
+    <t>M14</t>
+  </si>
+  <si>
+    <t>All pions and an equal amount of electrons, Scaled as follows: x=x/max(x)</t>
   </si>
 </sst>
 </file>
@@ -962,11 +971,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D847C349-F495-423A-9F1C-FAD29C38B92F}">
-  <dimension ref="A1:S129"/>
+  <dimension ref="A1:S153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S112" sqref="S112:S129"/>
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A154" sqref="A154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6274,6 +6283,1104 @@
       </c>
       <c r="S129" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>55</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130" t="b">
+        <v>1</v>
+      </c>
+      <c r="D130">
+        <v>32</v>
+      </c>
+      <c r="E130" t="s">
+        <v>19</v>
+      </c>
+      <c r="F130" t="b">
+        <v>1</v>
+      </c>
+      <c r="I130" t="s">
+        <v>27</v>
+      </c>
+      <c r="J130" t="s">
+        <v>5</v>
+      </c>
+      <c r="K130">
+        <v>32</v>
+      </c>
+      <c r="L130">
+        <v>0.01</v>
+      </c>
+      <c r="M130">
+        <v>0.9</v>
+      </c>
+      <c r="N130">
+        <v>50</v>
+      </c>
+      <c r="O130">
+        <v>0.62</v>
+      </c>
+      <c r="P130">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q130">
+        <v>0.9</v>
+      </c>
+      <c r="R130">
+        <v>0.88</v>
+      </c>
+      <c r="S130" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>55</v>
+      </c>
+      <c r="B131">
+        <v>2</v>
+      </c>
+      <c r="C131" t="b">
+        <v>1</v>
+      </c>
+      <c r="D131">
+        <v>64</v>
+      </c>
+      <c r="E131" t="s">
+        <v>19</v>
+      </c>
+      <c r="F131" t="b">
+        <v>1</v>
+      </c>
+      <c r="I131" t="s">
+        <v>27</v>
+      </c>
+      <c r="J131" t="s">
+        <v>5</v>
+      </c>
+      <c r="K131">
+        <v>32</v>
+      </c>
+      <c r="L131">
+        <v>0.01</v>
+      </c>
+      <c r="M131">
+        <v>0.9</v>
+      </c>
+      <c r="N131">
+        <v>50</v>
+      </c>
+      <c r="O131">
+        <v>0.62</v>
+      </c>
+      <c r="P131">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q131">
+        <v>0.9</v>
+      </c>
+      <c r="R131">
+        <v>0.88</v>
+      </c>
+      <c r="S131" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>55</v>
+      </c>
+      <c r="B132">
+        <v>3</v>
+      </c>
+      <c r="C132" t="b">
+        <v>1</v>
+      </c>
+      <c r="D132">
+        <v>128</v>
+      </c>
+      <c r="E132" t="s">
+        <v>30</v>
+      </c>
+      <c r="I132" t="s">
+        <v>27</v>
+      </c>
+      <c r="J132" t="s">
+        <v>5</v>
+      </c>
+      <c r="K132">
+        <v>32</v>
+      </c>
+      <c r="L132">
+        <v>0.01</v>
+      </c>
+      <c r="M132">
+        <v>0.9</v>
+      </c>
+      <c r="N132">
+        <v>50</v>
+      </c>
+      <c r="O132">
+        <v>0.62</v>
+      </c>
+      <c r="P132">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q132">
+        <v>0.9</v>
+      </c>
+      <c r="R132">
+        <v>0.88</v>
+      </c>
+      <c r="S132" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>55</v>
+      </c>
+      <c r="B133">
+        <v>4</v>
+      </c>
+      <c r="H133">
+        <v>256</v>
+      </c>
+      <c r="I133" t="s">
+        <v>33</v>
+      </c>
+      <c r="J133" t="s">
+        <v>5</v>
+      </c>
+      <c r="K133">
+        <v>32</v>
+      </c>
+      <c r="L133">
+        <v>0.01</v>
+      </c>
+      <c r="M133">
+        <v>0.9</v>
+      </c>
+      <c r="N133">
+        <v>50</v>
+      </c>
+      <c r="O133">
+        <v>0.62</v>
+      </c>
+      <c r="P133">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q133">
+        <v>0.9</v>
+      </c>
+      <c r="R133">
+        <v>0.88</v>
+      </c>
+      <c r="S133" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>55</v>
+      </c>
+      <c r="B134">
+        <v>5</v>
+      </c>
+      <c r="H134">
+        <v>128</v>
+      </c>
+      <c r="I134" t="s">
+        <v>33</v>
+      </c>
+      <c r="J134" t="s">
+        <v>5</v>
+      </c>
+      <c r="K134">
+        <v>32</v>
+      </c>
+      <c r="L134">
+        <v>0.01</v>
+      </c>
+      <c r="M134">
+        <v>0.9</v>
+      </c>
+      <c r="N134">
+        <v>50</v>
+      </c>
+      <c r="O134">
+        <v>0.62</v>
+      </c>
+      <c r="P134">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q134">
+        <v>0.9</v>
+      </c>
+      <c r="R134">
+        <v>0.88</v>
+      </c>
+      <c r="S134" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>55</v>
+      </c>
+      <c r="B135">
+        <v>6</v>
+      </c>
+      <c r="H135">
+        <v>128</v>
+      </c>
+      <c r="I135" t="s">
+        <v>33</v>
+      </c>
+      <c r="J135" t="s">
+        <v>5</v>
+      </c>
+      <c r="K135">
+        <v>32</v>
+      </c>
+      <c r="L135">
+        <v>0.01</v>
+      </c>
+      <c r="M135">
+        <v>0.9</v>
+      </c>
+      <c r="N135">
+        <v>50</v>
+      </c>
+      <c r="O135">
+        <v>0.62</v>
+      </c>
+      <c r="P135">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q135">
+        <v>0.9</v>
+      </c>
+      <c r="R135">
+        <v>0.88</v>
+      </c>
+      <c r="S135" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>55</v>
+      </c>
+      <c r="B136">
+        <v>7</v>
+      </c>
+      <c r="H136">
+        <v>64</v>
+      </c>
+      <c r="I136" t="s">
+        <v>33</v>
+      </c>
+      <c r="J136" t="s">
+        <v>5</v>
+      </c>
+      <c r="K136">
+        <v>32</v>
+      </c>
+      <c r="L136">
+        <v>0.01</v>
+      </c>
+      <c r="M136">
+        <v>0.9</v>
+      </c>
+      <c r="N136">
+        <v>50</v>
+      </c>
+      <c r="O136">
+        <v>0.62</v>
+      </c>
+      <c r="P136">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q136">
+        <v>0.9</v>
+      </c>
+      <c r="R136">
+        <v>0.88</v>
+      </c>
+      <c r="S136" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>55</v>
+      </c>
+      <c r="B137">
+        <v>8</v>
+      </c>
+      <c r="H137">
+        <v>32</v>
+      </c>
+      <c r="I137" t="s">
+        <v>33</v>
+      </c>
+      <c r="J137" t="s">
+        <v>5</v>
+      </c>
+      <c r="K137">
+        <v>32</v>
+      </c>
+      <c r="L137">
+        <v>0.01</v>
+      </c>
+      <c r="M137">
+        <v>0.9</v>
+      </c>
+      <c r="N137">
+        <v>50</v>
+      </c>
+      <c r="O137">
+        <v>0.62</v>
+      </c>
+      <c r="P137">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q137">
+        <v>0.9</v>
+      </c>
+      <c r="R137">
+        <v>0.88</v>
+      </c>
+      <c r="S137" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>55</v>
+      </c>
+      <c r="B138">
+        <v>9</v>
+      </c>
+      <c r="H138">
+        <v>2</v>
+      </c>
+      <c r="I138" t="s">
+        <v>26</v>
+      </c>
+      <c r="J138" t="s">
+        <v>5</v>
+      </c>
+      <c r="K138">
+        <v>32</v>
+      </c>
+      <c r="L138">
+        <v>0.01</v>
+      </c>
+      <c r="M138">
+        <v>0.9</v>
+      </c>
+      <c r="N138">
+        <v>50</v>
+      </c>
+      <c r="O138">
+        <v>0.62</v>
+      </c>
+      <c r="P138">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q138">
+        <v>0.9</v>
+      </c>
+      <c r="R138">
+        <v>0.88</v>
+      </c>
+      <c r="S138" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>56</v>
+      </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
+      <c r="C139" t="b">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <v>32</v>
+      </c>
+      <c r="E139" t="s">
+        <v>19</v>
+      </c>
+      <c r="F139" t="b">
+        <v>1</v>
+      </c>
+      <c r="I139" t="s">
+        <v>33</v>
+      </c>
+      <c r="J139" t="s">
+        <v>5</v>
+      </c>
+      <c r="K139">
+        <v>32</v>
+      </c>
+      <c r="L139">
+        <v>0.01</v>
+      </c>
+      <c r="M139">
+        <v>0.9</v>
+      </c>
+      <c r="N139">
+        <v>50</v>
+      </c>
+      <c r="O139">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P139">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q139">
+        <v>0.9</v>
+      </c>
+      <c r="R139">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S139" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>56</v>
+      </c>
+      <c r="B140">
+        <v>2</v>
+      </c>
+      <c r="C140" t="b">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>64</v>
+      </c>
+      <c r="E140" t="s">
+        <v>19</v>
+      </c>
+      <c r="F140" t="b">
+        <v>1</v>
+      </c>
+      <c r="I140" t="s">
+        <v>33</v>
+      </c>
+      <c r="J140" t="s">
+        <v>5</v>
+      </c>
+      <c r="K140">
+        <v>32</v>
+      </c>
+      <c r="L140">
+        <v>0.01</v>
+      </c>
+      <c r="M140">
+        <v>0.9</v>
+      </c>
+      <c r="N140">
+        <v>50</v>
+      </c>
+      <c r="O140">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P140">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q140">
+        <v>0.9</v>
+      </c>
+      <c r="R140">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S140" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>56</v>
+      </c>
+      <c r="B141">
+        <v>3</v>
+      </c>
+      <c r="H141">
+        <v>1024</v>
+      </c>
+      <c r="I141" t="s">
+        <v>33</v>
+      </c>
+      <c r="J141" t="s">
+        <v>5</v>
+      </c>
+      <c r="K141">
+        <v>32</v>
+      </c>
+      <c r="L141">
+        <v>0.01</v>
+      </c>
+      <c r="M141">
+        <v>0.9</v>
+      </c>
+      <c r="N141">
+        <v>50</v>
+      </c>
+      <c r="O141">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P141">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q141">
+        <v>0.9</v>
+      </c>
+      <c r="R141">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S141" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>56</v>
+      </c>
+      <c r="B142">
+        <v>4</v>
+      </c>
+      <c r="H142">
+        <v>1024</v>
+      </c>
+      <c r="I142" t="s">
+        <v>33</v>
+      </c>
+      <c r="J142" t="s">
+        <v>5</v>
+      </c>
+      <c r="K142">
+        <v>32</v>
+      </c>
+      <c r="L142">
+        <v>0.01</v>
+      </c>
+      <c r="M142">
+        <v>0.9</v>
+      </c>
+      <c r="N142">
+        <v>50</v>
+      </c>
+      <c r="O142">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P142">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q142">
+        <v>0.9</v>
+      </c>
+      <c r="R142">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S142" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>56</v>
+      </c>
+      <c r="B143">
+        <v>5</v>
+      </c>
+      <c r="H143">
+        <v>512</v>
+      </c>
+      <c r="I143" t="s">
+        <v>4</v>
+      </c>
+      <c r="J143" t="s">
+        <v>5</v>
+      </c>
+      <c r="K143">
+        <v>32</v>
+      </c>
+      <c r="L143">
+        <v>0.01</v>
+      </c>
+      <c r="M143">
+        <v>0.9</v>
+      </c>
+      <c r="N143">
+        <v>50</v>
+      </c>
+      <c r="O143">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P143">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q143">
+        <v>0.9</v>
+      </c>
+      <c r="R143">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S143" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>56</v>
+      </c>
+      <c r="B144">
+        <v>6</v>
+      </c>
+      <c r="H144">
+        <v>512</v>
+      </c>
+      <c r="I144" t="s">
+        <v>4</v>
+      </c>
+      <c r="J144" t="s">
+        <v>5</v>
+      </c>
+      <c r="K144">
+        <v>32</v>
+      </c>
+      <c r="L144">
+        <v>0.01</v>
+      </c>
+      <c r="M144">
+        <v>0.9</v>
+      </c>
+      <c r="N144">
+        <v>50</v>
+      </c>
+      <c r="O144">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P144">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q144">
+        <v>0.9</v>
+      </c>
+      <c r="R144">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S144" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>56</v>
+      </c>
+      <c r="B145">
+        <v>7</v>
+      </c>
+      <c r="H145">
+        <v>256</v>
+      </c>
+      <c r="I145" t="s">
+        <v>4</v>
+      </c>
+      <c r="J145" t="s">
+        <v>5</v>
+      </c>
+      <c r="K145">
+        <v>32</v>
+      </c>
+      <c r="L145">
+        <v>0.01</v>
+      </c>
+      <c r="M145">
+        <v>0.9</v>
+      </c>
+      <c r="N145">
+        <v>50</v>
+      </c>
+      <c r="O145">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P145">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q145">
+        <v>0.9</v>
+      </c>
+      <c r="R145">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S145" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>56</v>
+      </c>
+      <c r="B146">
+        <v>8</v>
+      </c>
+      <c r="H146">
+        <v>256</v>
+      </c>
+      <c r="I146" t="s">
+        <v>4</v>
+      </c>
+      <c r="J146" t="s">
+        <v>5</v>
+      </c>
+      <c r="K146">
+        <v>32</v>
+      </c>
+      <c r="L146">
+        <v>0.01</v>
+      </c>
+      <c r="M146">
+        <v>0.9</v>
+      </c>
+      <c r="N146">
+        <v>50</v>
+      </c>
+      <c r="O146">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P146">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q146">
+        <v>0.9</v>
+      </c>
+      <c r="R146">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S146" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>56</v>
+      </c>
+      <c r="B147">
+        <v>9</v>
+      </c>
+      <c r="H147">
+        <v>256</v>
+      </c>
+      <c r="I147" t="s">
+        <v>4</v>
+      </c>
+      <c r="J147" t="s">
+        <v>5</v>
+      </c>
+      <c r="K147">
+        <v>32</v>
+      </c>
+      <c r="L147">
+        <v>0.01</v>
+      </c>
+      <c r="M147">
+        <v>0.9</v>
+      </c>
+      <c r="N147">
+        <v>50</v>
+      </c>
+      <c r="O147">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P147">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q147">
+        <v>0.9</v>
+      </c>
+      <c r="R147">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S147" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>56</v>
+      </c>
+      <c r="B148">
+        <v>10</v>
+      </c>
+      <c r="H148">
+        <v>256</v>
+      </c>
+      <c r="I148" t="s">
+        <v>4</v>
+      </c>
+      <c r="J148" t="s">
+        <v>5</v>
+      </c>
+      <c r="K148">
+        <v>32</v>
+      </c>
+      <c r="L148">
+        <v>0.01</v>
+      </c>
+      <c r="M148">
+        <v>0.9</v>
+      </c>
+      <c r="N148">
+        <v>50</v>
+      </c>
+      <c r="O148">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P148">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q148">
+        <v>0.9</v>
+      </c>
+      <c r="R148">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S148" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>56</v>
+      </c>
+      <c r="B149">
+        <v>11</v>
+      </c>
+      <c r="H149">
+        <v>128</v>
+      </c>
+      <c r="I149" t="s">
+        <v>4</v>
+      </c>
+      <c r="J149" t="s">
+        <v>5</v>
+      </c>
+      <c r="K149">
+        <v>32</v>
+      </c>
+      <c r="L149">
+        <v>0.01</v>
+      </c>
+      <c r="M149">
+        <v>0.9</v>
+      </c>
+      <c r="N149">
+        <v>50</v>
+      </c>
+      <c r="O149">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P149">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q149">
+        <v>0.9</v>
+      </c>
+      <c r="R149">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S149" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>56</v>
+      </c>
+      <c r="B150">
+        <v>12</v>
+      </c>
+      <c r="H150">
+        <v>64</v>
+      </c>
+      <c r="I150" t="s">
+        <v>4</v>
+      </c>
+      <c r="J150" t="s">
+        <v>5</v>
+      </c>
+      <c r="K150">
+        <v>32</v>
+      </c>
+      <c r="L150">
+        <v>0.01</v>
+      </c>
+      <c r="M150">
+        <v>0.9</v>
+      </c>
+      <c r="N150">
+        <v>50</v>
+      </c>
+      <c r="O150">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P150">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q150">
+        <v>0.9</v>
+      </c>
+      <c r="R150">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S150" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>56</v>
+      </c>
+      <c r="B151">
+        <v>13</v>
+      </c>
+      <c r="H151">
+        <v>64</v>
+      </c>
+      <c r="I151" t="s">
+        <v>4</v>
+      </c>
+      <c r="J151" t="s">
+        <v>5</v>
+      </c>
+      <c r="K151">
+        <v>32</v>
+      </c>
+      <c r="L151">
+        <v>0.01</v>
+      </c>
+      <c r="M151">
+        <v>0.9</v>
+      </c>
+      <c r="N151">
+        <v>50</v>
+      </c>
+      <c r="O151">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P151">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q151">
+        <v>0.9</v>
+      </c>
+      <c r="R151">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S151" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>56</v>
+      </c>
+      <c r="B152">
+        <v>14</v>
+      </c>
+      <c r="H152">
+        <v>32</v>
+      </c>
+      <c r="I152" t="s">
+        <v>4</v>
+      </c>
+      <c r="J152" t="s">
+        <v>5</v>
+      </c>
+      <c r="K152">
+        <v>32</v>
+      </c>
+      <c r="L152">
+        <v>0.01</v>
+      </c>
+      <c r="M152">
+        <v>0.9</v>
+      </c>
+      <c r="N152">
+        <v>50</v>
+      </c>
+      <c r="O152">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P152">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q152">
+        <v>0.9</v>
+      </c>
+      <c r="R152">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S152" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>56</v>
+      </c>
+      <c r="B153">
+        <v>15</v>
+      </c>
+      <c r="H153">
+        <v>2</v>
+      </c>
+      <c r="I153" t="s">
+        <v>26</v>
+      </c>
+      <c r="J153" t="s">
+        <v>5</v>
+      </c>
+      <c r="K153">
+        <v>32</v>
+      </c>
+      <c r="L153">
+        <v>0.01</v>
+      </c>
+      <c r="M153">
+        <v>0.9</v>
+      </c>
+      <c r="N153">
+        <v>50</v>
+      </c>
+      <c r="O153">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P153">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q153">
+        <v>0.9</v>
+      </c>
+      <c r="R153">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S153" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -6744,10 +7851,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98088B90-BB92-4A82-86B2-658E03FA1477}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6800,6 +7907,26 @@
         <v>54</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>10000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3">
+        <v>0.9</v>
+      </c>
+      <c r="E3">
+        <v>0.79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
All chamber-gain corrected models added to assessment of models
</commit_message>
<xml_diff>
--- a/NEW/statistical_analysis/Networks Compared.xlsx
+++ b/NEW/statistical_analysis/Networks Compared.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerhard\Documents\MSc-thesis\NEW\statistical_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A45C5C-86BF-40AF-83DA-5ADCB14917B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95ED5591-A72C-4D4C-951C-22EAE7839BA0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="-120" windowWidth="27300" windowHeight="16440" activeTab="2" xr2:uid="{42FDFE43-F33F-4893-BA97-B5C32084F215}"/>
+    <workbookView xWindow="1620" yWindow="-120" windowWidth="27300" windowHeight="16440" xr2:uid="{42FDFE43-F33F-4893-BA97-B5C32084F215}"/>
   </bookViews>
   <sheets>
     <sheet name="Fully conected" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2447" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2707" uniqueCount="118">
   <si>
     <t>Model Number</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>Column Sums, Chamber Gain Corrected, tracks that have 6 tracklets, all electrons and an equal number of pions, scaled as follows: x=x/max(x)</t>
+  </si>
+  <si>
+    <t>Column Sums, Mean Pixel Value, Standard deviation pixel value,l2 norm of image, max pixel value, 6 timebins summed sequentially, lagged differences of 6-column sums with lag=1, Chamber Gain Corrected, tracks that have 6 tracklets, all electrons and an equal number of pions, scaled as follows: x=x/max(x)</t>
   </si>
 </sst>
 </file>
@@ -761,11 +764,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32EF017-127E-4272-A45C-8B2FC1D130CC}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +787,7 @@
     <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="154.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="62.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -1137,6 +1140,355 @@
       </c>
       <c r="P8" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
+        <v>1024</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9">
+        <v>32</v>
+      </c>
+      <c r="H9">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K9">
+        <v>100</v>
+      </c>
+      <c r="L9">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="M9">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="N9">
+        <v>0.9</v>
+      </c>
+      <c r="O9">
+        <v>0.14863999999999999</v>
+      </c>
+      <c r="P9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>512</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10">
+        <v>32</v>
+      </c>
+      <c r="H10">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K10">
+        <v>100</v>
+      </c>
+      <c r="L10">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="M10">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="N10">
+        <v>0.9</v>
+      </c>
+      <c r="O10">
+        <v>0.14863999999999999</v>
+      </c>
+      <c r="P10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11">
+        <v>256</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11">
+        <v>32</v>
+      </c>
+      <c r="H11">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K11">
+        <v>100</v>
+      </c>
+      <c r="L11">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="M11">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="N11">
+        <v>0.9</v>
+      </c>
+      <c r="O11">
+        <v>0.14863999999999999</v>
+      </c>
+      <c r="P11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <v>128</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12">
+        <v>32</v>
+      </c>
+      <c r="H12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K12">
+        <v>100</v>
+      </c>
+      <c r="L12">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="M12">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="N12">
+        <v>0.9</v>
+      </c>
+      <c r="O12">
+        <v>0.14863999999999999</v>
+      </c>
+      <c r="P12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="D13">
+        <v>128</v>
+      </c>
+      <c r="E13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13">
+        <v>32</v>
+      </c>
+      <c r="H13">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K13">
+        <v>100</v>
+      </c>
+      <c r="L13">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="M13">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="N13">
+        <v>0.9</v>
+      </c>
+      <c r="O13">
+        <v>0.14863999999999999</v>
+      </c>
+      <c r="P13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="D14">
+        <v>128</v>
+      </c>
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14">
+        <v>32</v>
+      </c>
+      <c r="H14">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="L14">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="M14">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="N14">
+        <v>0.9</v>
+      </c>
+      <c r="O14">
+        <v>0.14863999999999999</v>
+      </c>
+      <c r="P14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>0.5</v>
+      </c>
+      <c r="D15">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15">
+        <v>32</v>
+      </c>
+      <c r="H15">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K15">
+        <v>100</v>
+      </c>
+      <c r="L15">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="M15">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="N15">
+        <v>0.9</v>
+      </c>
+      <c r="O15">
+        <v>0.14863999999999999</v>
+      </c>
+      <c r="P15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16">
+        <v>32</v>
+      </c>
+      <c r="H16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
+      </c>
+      <c r="L16">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="M16">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="N16">
+        <v>0.9</v>
+      </c>
+      <c r="O16">
+        <v>0.14863999999999999</v>
+      </c>
+      <c r="P16" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1150,7 +1502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D847C349-F495-423A-9F1C-FAD29C38B92F}">
   <dimension ref="A1:W372"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A354" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="W370" sqref="W370"/>
     </sheetView>
@@ -18562,10 +18914,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4356D11A-C020-4F7F-859E-F8F25B3322AC}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19594,6 +19947,1167 @@
       <c r="A22" t="s">
         <v>13</v>
       </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" t="s">
+        <v>76</v>
+      </c>
+      <c r="L22" t="s">
+        <v>70</v>
+      </c>
+      <c r="M22">
+        <v>32</v>
+      </c>
+      <c r="N22">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P22">
+        <v>100</v>
+      </c>
+      <c r="Q22">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R22">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="S22">
+        <v>0.9</v>
+      </c>
+      <c r="T22">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="U22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" t="s">
+        <v>76</v>
+      </c>
+      <c r="L23" t="s">
+        <v>70</v>
+      </c>
+      <c r="M23">
+        <v>32</v>
+      </c>
+      <c r="N23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P23">
+        <v>100</v>
+      </c>
+      <c r="Q23">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R23">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="S23">
+        <v>0.9</v>
+      </c>
+      <c r="T23">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="U23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>24</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" t="s">
+        <v>76</v>
+      </c>
+      <c r="L24" t="s">
+        <v>70</v>
+      </c>
+      <c r="M24">
+        <v>32</v>
+      </c>
+      <c r="N24">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P24">
+        <v>100</v>
+      </c>
+      <c r="Q24">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R24">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="S24">
+        <v>0.9</v>
+      </c>
+      <c r="T24">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="U24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>48</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="J25" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" t="s">
+        <v>76</v>
+      </c>
+      <c r="L25" t="s">
+        <v>70</v>
+      </c>
+      <c r="M25">
+        <v>32</v>
+      </c>
+      <c r="N25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P25">
+        <v>100</v>
+      </c>
+      <c r="Q25">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R25">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="S25">
+        <v>0.9</v>
+      </c>
+      <c r="T25">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="U25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="H26">
+        <v>512</v>
+      </c>
+      <c r="J26" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" t="s">
+        <v>76</v>
+      </c>
+      <c r="L26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M26">
+        <v>32</v>
+      </c>
+      <c r="N26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P26">
+        <v>100</v>
+      </c>
+      <c r="Q26">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R26">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="S26">
+        <v>0.9</v>
+      </c>
+      <c r="T26">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="U26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="H27">
+        <v>512</v>
+      </c>
+      <c r="J27" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" t="s">
+        <v>76</v>
+      </c>
+      <c r="L27" t="s">
+        <v>70</v>
+      </c>
+      <c r="M27">
+        <v>32</v>
+      </c>
+      <c r="N27">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P27">
+        <v>100</v>
+      </c>
+      <c r="Q27">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R27">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="S27">
+        <v>0.9</v>
+      </c>
+      <c r="T27">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="U27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="H28">
+        <v>256</v>
+      </c>
+      <c r="J28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" t="s">
+        <v>76</v>
+      </c>
+      <c r="L28" t="s">
+        <v>70</v>
+      </c>
+      <c r="M28">
+        <v>32</v>
+      </c>
+      <c r="N28">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P28">
+        <v>100</v>
+      </c>
+      <c r="Q28">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R28">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="S28">
+        <v>0.9</v>
+      </c>
+      <c r="T28">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="U28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="H29">
+        <v>256</v>
+      </c>
+      <c r="J29" t="s">
+        <v>33</v>
+      </c>
+      <c r="K29" t="s">
+        <v>76</v>
+      </c>
+      <c r="L29" t="s">
+        <v>70</v>
+      </c>
+      <c r="M29">
+        <v>32</v>
+      </c>
+      <c r="N29">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P29">
+        <v>100</v>
+      </c>
+      <c r="Q29">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R29">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="S29">
+        <v>0.9</v>
+      </c>
+      <c r="T29">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="U29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30">
+        <v>9</v>
+      </c>
+      <c r="H30">
+        <v>128</v>
+      </c>
+      <c r="J30" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" t="s">
+        <v>76</v>
+      </c>
+      <c r="L30" t="s">
+        <v>70</v>
+      </c>
+      <c r="M30">
+        <v>32</v>
+      </c>
+      <c r="N30">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P30">
+        <v>100</v>
+      </c>
+      <c r="Q30">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R30">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="S30">
+        <v>0.9</v>
+      </c>
+      <c r="T30">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="U30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="H31">
+        <v>128</v>
+      </c>
+      <c r="J31" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" t="s">
+        <v>76</v>
+      </c>
+      <c r="L31" t="s">
+        <v>70</v>
+      </c>
+      <c r="M31">
+        <v>32</v>
+      </c>
+      <c r="N31">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P31">
+        <v>100</v>
+      </c>
+      <c r="Q31">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R31">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="S31">
+        <v>0.9</v>
+      </c>
+      <c r="T31">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="U31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32">
+        <v>11</v>
+      </c>
+      <c r="H32">
+        <v>64</v>
+      </c>
+      <c r="J32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L32" t="s">
+        <v>70</v>
+      </c>
+      <c r="M32">
+        <v>32</v>
+      </c>
+      <c r="N32">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P32">
+        <v>100</v>
+      </c>
+      <c r="Q32">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R32">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="S32">
+        <v>0.9</v>
+      </c>
+      <c r="T32">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="U32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33">
+        <v>12</v>
+      </c>
+      <c r="H33">
+        <v>32</v>
+      </c>
+      <c r="J33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33" t="s">
+        <v>76</v>
+      </c>
+      <c r="L33" t="s">
+        <v>70</v>
+      </c>
+      <c r="M33">
+        <v>32</v>
+      </c>
+      <c r="N33">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P33">
+        <v>100</v>
+      </c>
+      <c r="Q33">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R33">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="S33">
+        <v>0.9</v>
+      </c>
+      <c r="T33">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="U33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34">
+        <v>13</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>69</v>
+      </c>
+      <c r="K34" t="s">
+        <v>76</v>
+      </c>
+      <c r="L34" t="s">
+        <v>70</v>
+      </c>
+      <c r="M34">
+        <v>32</v>
+      </c>
+      <c r="N34">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P34">
+        <v>100</v>
+      </c>
+      <c r="Q34">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R34">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="S34">
+        <v>0.9</v>
+      </c>
+      <c r="T34">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="U34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>32</v>
+      </c>
+      <c r="E35">
+        <v>6</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>27</v>
+      </c>
+      <c r="K35" t="s">
+        <v>76</v>
+      </c>
+      <c r="L35" t="s">
+        <v>70</v>
+      </c>
+      <c r="M35">
+        <v>32</v>
+      </c>
+      <c r="N35">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P35">
+        <v>100</v>
+      </c>
+      <c r="Q35">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="R35">
+        <v>0.72</v>
+      </c>
+      <c r="S35">
+        <v>0.9</v>
+      </c>
+      <c r="T35">
+        <v>8.9870000000000005E-2</v>
+      </c>
+      <c r="U35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>64</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
+        <v>27</v>
+      </c>
+      <c r="K36" t="s">
+        <v>76</v>
+      </c>
+      <c r="L36" t="s">
+        <v>70</v>
+      </c>
+      <c r="M36">
+        <v>32</v>
+      </c>
+      <c r="N36">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P36">
+        <v>100</v>
+      </c>
+      <c r="Q36">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="R36">
+        <v>0.72</v>
+      </c>
+      <c r="S36">
+        <v>0.9</v>
+      </c>
+      <c r="T36">
+        <v>8.9870000000000005E-2</v>
+      </c>
+      <c r="U36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>128</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>27</v>
+      </c>
+      <c r="K37" t="s">
+        <v>76</v>
+      </c>
+      <c r="L37" t="s">
+        <v>70</v>
+      </c>
+      <c r="M37">
+        <v>32</v>
+      </c>
+      <c r="N37">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P37">
+        <v>100</v>
+      </c>
+      <c r="Q37">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="R37">
+        <v>0.72</v>
+      </c>
+      <c r="S37">
+        <v>0.9</v>
+      </c>
+      <c r="T37">
+        <v>8.9870000000000005E-2</v>
+      </c>
+      <c r="U37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>512</v>
+      </c>
+      <c r="J38" t="s">
+        <v>33</v>
+      </c>
+      <c r="K38" t="s">
+        <v>76</v>
+      </c>
+      <c r="L38" t="s">
+        <v>70</v>
+      </c>
+      <c r="M38">
+        <v>32</v>
+      </c>
+      <c r="N38">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P38">
+        <v>100</v>
+      </c>
+      <c r="Q38">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="R38">
+        <v>0.72</v>
+      </c>
+      <c r="S38">
+        <v>0.9</v>
+      </c>
+      <c r="T38">
+        <v>8.9870000000000005E-2</v>
+      </c>
+      <c r="U38" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="H39">
+        <v>512</v>
+      </c>
+      <c r="J39" t="s">
+        <v>33</v>
+      </c>
+      <c r="K39" t="s">
+        <v>76</v>
+      </c>
+      <c r="L39" t="s">
+        <v>70</v>
+      </c>
+      <c r="M39">
+        <v>32</v>
+      </c>
+      <c r="N39">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P39">
+        <v>100</v>
+      </c>
+      <c r="Q39">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="R39">
+        <v>0.72</v>
+      </c>
+      <c r="S39">
+        <v>0.9</v>
+      </c>
+      <c r="T39">
+        <v>8.9870000000000005E-2</v>
+      </c>
+      <c r="U39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="H40">
+        <v>256</v>
+      </c>
+      <c r="J40" t="s">
+        <v>33</v>
+      </c>
+      <c r="K40" t="s">
+        <v>76</v>
+      </c>
+      <c r="L40" t="s">
+        <v>70</v>
+      </c>
+      <c r="M40">
+        <v>32</v>
+      </c>
+      <c r="N40">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P40">
+        <v>100</v>
+      </c>
+      <c r="Q40">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="R40">
+        <v>0.72</v>
+      </c>
+      <c r="S40">
+        <v>0.9</v>
+      </c>
+      <c r="T40">
+        <v>8.9870000000000005E-2</v>
+      </c>
+      <c r="U40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+      <c r="H41">
+        <v>256</v>
+      </c>
+      <c r="J41" t="s">
+        <v>33</v>
+      </c>
+      <c r="K41" t="s">
+        <v>76</v>
+      </c>
+      <c r="L41" t="s">
+        <v>70</v>
+      </c>
+      <c r="M41">
+        <v>32</v>
+      </c>
+      <c r="N41">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P41">
+        <v>100</v>
+      </c>
+      <c r="Q41">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="R41">
+        <v>0.72</v>
+      </c>
+      <c r="S41">
+        <v>0.9</v>
+      </c>
+      <c r="T41">
+        <v>8.9870000000000005E-2</v>
+      </c>
+      <c r="U41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="H42">
+        <v>128</v>
+      </c>
+      <c r="J42" t="s">
+        <v>33</v>
+      </c>
+      <c r="K42" t="s">
+        <v>76</v>
+      </c>
+      <c r="L42" t="s">
+        <v>70</v>
+      </c>
+      <c r="M42">
+        <v>32</v>
+      </c>
+      <c r="N42">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P42">
+        <v>100</v>
+      </c>
+      <c r="Q42">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="R42">
+        <v>0.72</v>
+      </c>
+      <c r="S42">
+        <v>0.9</v>
+      </c>
+      <c r="T42">
+        <v>8.9870000000000005E-2</v>
+      </c>
+      <c r="U42" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43">
+        <v>9</v>
+      </c>
+      <c r="H43">
+        <v>128</v>
+      </c>
+      <c r="J43" t="s">
+        <v>33</v>
+      </c>
+      <c r="K43" t="s">
+        <v>76</v>
+      </c>
+      <c r="L43" t="s">
+        <v>70</v>
+      </c>
+      <c r="M43">
+        <v>32</v>
+      </c>
+      <c r="N43">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P43">
+        <v>100</v>
+      </c>
+      <c r="Q43">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="R43">
+        <v>0.72</v>
+      </c>
+      <c r="S43">
+        <v>0.9</v>
+      </c>
+      <c r="T43">
+        <v>8.9870000000000005E-2</v>
+      </c>
+      <c r="U43" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
+      </c>
+      <c r="H44">
+        <v>64</v>
+      </c>
+      <c r="J44" t="s">
+        <v>33</v>
+      </c>
+      <c r="K44" t="s">
+        <v>76</v>
+      </c>
+      <c r="L44" t="s">
+        <v>70</v>
+      </c>
+      <c r="M44">
+        <v>32</v>
+      </c>
+      <c r="N44">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P44">
+        <v>100</v>
+      </c>
+      <c r="Q44">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="R44">
+        <v>0.72</v>
+      </c>
+      <c r="S44">
+        <v>0.9</v>
+      </c>
+      <c r="T44">
+        <v>8.9870000000000005E-2</v>
+      </c>
+      <c r="U44" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45">
+        <v>11</v>
+      </c>
+      <c r="H45">
+        <v>32</v>
+      </c>
+      <c r="J45" t="s">
+        <v>33</v>
+      </c>
+      <c r="K45" t="s">
+        <v>76</v>
+      </c>
+      <c r="L45" t="s">
+        <v>70</v>
+      </c>
+      <c r="M45">
+        <v>32</v>
+      </c>
+      <c r="N45">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P45">
+        <v>100</v>
+      </c>
+      <c r="Q45">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="R45">
+        <v>0.72</v>
+      </c>
+      <c r="S45">
+        <v>0.9</v>
+      </c>
+      <c r="T45">
+        <v>8.9870000000000005E-2</v>
+      </c>
+      <c r="U45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46">
+        <v>12</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+      <c r="J46" t="s">
+        <v>69</v>
+      </c>
+      <c r="K46" t="s">
+        <v>76</v>
+      </c>
+      <c r="L46" t="s">
+        <v>70</v>
+      </c>
+      <c r="M46">
+        <v>32</v>
+      </c>
+      <c r="N46">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P46">
+        <v>100</v>
+      </c>
+      <c r="Q46">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="R46">
+        <v>0.72</v>
+      </c>
+      <c r="S46">
+        <v>0.9</v>
+      </c>
+      <c r="T46">
+        <v>8.9870000000000005E-2</v>
+      </c>
+      <c r="U46" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -19603,12 +21117,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26382EEA-56AD-452C-9D78-7AC7571B137C}">
-  <dimension ref="A1:R69"/>
+  <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
+      <selection pane="bottomLeft" activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22649,6 +24163,1102 @@
         <v>9.2350000000000002E-2</v>
       </c>
       <c r="R69" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="b">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>128</v>
+      </c>
+      <c r="E70" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" t="s">
+        <v>27</v>
+      </c>
+      <c r="I70" t="s">
+        <v>70</v>
+      </c>
+      <c r="J70">
+        <v>32</v>
+      </c>
+      <c r="K70">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M70">
+        <v>100</v>
+      </c>
+      <c r="N70">
+        <v>0.74</v>
+      </c>
+      <c r="O70">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="P70">
+        <v>0.9</v>
+      </c>
+      <c r="Q70">
+        <v>5.8169999999999999E-2</v>
+      </c>
+      <c r="R70" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71" t="b">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>128</v>
+      </c>
+      <c r="E71" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" t="s">
+        <v>27</v>
+      </c>
+      <c r="I71" t="s">
+        <v>70</v>
+      </c>
+      <c r="J71">
+        <v>32</v>
+      </c>
+      <c r="K71">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M71">
+        <v>100</v>
+      </c>
+      <c r="N71">
+        <v>0.74</v>
+      </c>
+      <c r="O71">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="P71">
+        <v>0.9</v>
+      </c>
+      <c r="Q71">
+        <v>5.8169999999999999E-2</v>
+      </c>
+      <c r="R71" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72">
+        <v>3</v>
+      </c>
+      <c r="F72">
+        <v>128</v>
+      </c>
+      <c r="H72" t="s">
+        <v>33</v>
+      </c>
+      <c r="I72" t="s">
+        <v>70</v>
+      </c>
+      <c r="J72">
+        <v>32</v>
+      </c>
+      <c r="K72">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M72">
+        <v>100</v>
+      </c>
+      <c r="N72">
+        <v>0.74</v>
+      </c>
+      <c r="O72">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="P72">
+        <v>0.9</v>
+      </c>
+      <c r="Q72">
+        <v>5.8169999999999999E-2</v>
+      </c>
+      <c r="R72" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>42</v>
+      </c>
+      <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="F73">
+        <v>128</v>
+      </c>
+      <c r="H73" t="s">
+        <v>33</v>
+      </c>
+      <c r="I73" t="s">
+        <v>70</v>
+      </c>
+      <c r="J73">
+        <v>32</v>
+      </c>
+      <c r="K73">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M73">
+        <v>100</v>
+      </c>
+      <c r="N73">
+        <v>0.74</v>
+      </c>
+      <c r="O73">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="P73">
+        <v>0.9</v>
+      </c>
+      <c r="Q73">
+        <v>5.8169999999999999E-2</v>
+      </c>
+      <c r="R73" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>42</v>
+      </c>
+      <c r="B74">
+        <v>5</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="H74" t="s">
+        <v>69</v>
+      </c>
+      <c r="I74" t="s">
+        <v>70</v>
+      </c>
+      <c r="J74">
+        <v>32</v>
+      </c>
+      <c r="K74">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M74">
+        <v>100</v>
+      </c>
+      <c r="N74">
+        <v>0.74</v>
+      </c>
+      <c r="O74">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="P74">
+        <v>0.9</v>
+      </c>
+      <c r="Q74">
+        <v>5.8169999999999999E-2</v>
+      </c>
+      <c r="R74" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>44</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75" t="b">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>256</v>
+      </c>
+      <c r="E75" t="b">
+        <v>0</v>
+      </c>
+      <c r="H75" t="s">
+        <v>27</v>
+      </c>
+      <c r="I75" t="s">
+        <v>70</v>
+      </c>
+      <c r="J75">
+        <v>32</v>
+      </c>
+      <c r="K75">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M75">
+        <v>100</v>
+      </c>
+      <c r="N75">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="O75">
+        <v>0.74</v>
+      </c>
+      <c r="P75">
+        <v>0.9</v>
+      </c>
+      <c r="Q75">
+        <v>5.3019999999999998E-2</v>
+      </c>
+      <c r="R75" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>44</v>
+      </c>
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76" t="b">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>256</v>
+      </c>
+      <c r="E76" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76" t="s">
+        <v>27</v>
+      </c>
+      <c r="I76" t="s">
+        <v>70</v>
+      </c>
+      <c r="J76">
+        <v>32</v>
+      </c>
+      <c r="K76">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M76">
+        <v>100</v>
+      </c>
+      <c r="N76">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="O76">
+        <v>0.74</v>
+      </c>
+      <c r="P76">
+        <v>0.9</v>
+      </c>
+      <c r="Q76">
+        <v>5.3019999999999998E-2</v>
+      </c>
+      <c r="R76" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>44</v>
+      </c>
+      <c r="B77">
+        <v>3</v>
+      </c>
+      <c r="F77">
+        <v>256</v>
+      </c>
+      <c r="H77" t="s">
+        <v>33</v>
+      </c>
+      <c r="I77" t="s">
+        <v>70</v>
+      </c>
+      <c r="J77">
+        <v>32</v>
+      </c>
+      <c r="K77">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M77">
+        <v>100</v>
+      </c>
+      <c r="N77">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="O77">
+        <v>0.74</v>
+      </c>
+      <c r="P77">
+        <v>0.9</v>
+      </c>
+      <c r="Q77">
+        <v>5.3019999999999998E-2</v>
+      </c>
+      <c r="R77" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>44</v>
+      </c>
+      <c r="B78">
+        <v>4</v>
+      </c>
+      <c r="F78">
+        <v>256</v>
+      </c>
+      <c r="H78" t="s">
+        <v>33</v>
+      </c>
+      <c r="I78" t="s">
+        <v>70</v>
+      </c>
+      <c r="J78">
+        <v>32</v>
+      </c>
+      <c r="K78">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M78">
+        <v>100</v>
+      </c>
+      <c r="N78">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="O78">
+        <v>0.74</v>
+      </c>
+      <c r="P78">
+        <v>0.9</v>
+      </c>
+      <c r="Q78">
+        <v>5.3019999999999998E-2</v>
+      </c>
+      <c r="R78" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>44</v>
+      </c>
+      <c r="B79">
+        <v>5</v>
+      </c>
+      <c r="F79">
+        <v>256</v>
+      </c>
+      <c r="H79" t="s">
+        <v>33</v>
+      </c>
+      <c r="I79" t="s">
+        <v>70</v>
+      </c>
+      <c r="J79">
+        <v>32</v>
+      </c>
+      <c r="K79">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M79">
+        <v>100</v>
+      </c>
+      <c r="N79">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="O79">
+        <v>0.74</v>
+      </c>
+      <c r="P79">
+        <v>0.9</v>
+      </c>
+      <c r="Q79">
+        <v>5.3019999999999998E-2</v>
+      </c>
+      <c r="R79" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>44</v>
+      </c>
+      <c r="B80">
+        <v>6</v>
+      </c>
+      <c r="F80">
+        <v>128</v>
+      </c>
+      <c r="H80" t="s">
+        <v>33</v>
+      </c>
+      <c r="I80" t="s">
+        <v>70</v>
+      </c>
+      <c r="J80">
+        <v>32</v>
+      </c>
+      <c r="K80">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M80">
+        <v>100</v>
+      </c>
+      <c r="N80">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="O80">
+        <v>0.74</v>
+      </c>
+      <c r="P80">
+        <v>0.9</v>
+      </c>
+      <c r="Q80">
+        <v>5.3019999999999998E-2</v>
+      </c>
+      <c r="R80" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>44</v>
+      </c>
+      <c r="B81">
+        <v>7</v>
+      </c>
+      <c r="F81">
+        <v>128</v>
+      </c>
+      <c r="H81" t="s">
+        <v>33</v>
+      </c>
+      <c r="I81" t="s">
+        <v>70</v>
+      </c>
+      <c r="J81">
+        <v>32</v>
+      </c>
+      <c r="K81">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M81">
+        <v>100</v>
+      </c>
+      <c r="N81">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="O81">
+        <v>0.74</v>
+      </c>
+      <c r="P81">
+        <v>0.9</v>
+      </c>
+      <c r="Q81">
+        <v>5.3019999999999998E-2</v>
+      </c>
+      <c r="R81" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>44</v>
+      </c>
+      <c r="B82">
+        <v>8</v>
+      </c>
+      <c r="F82">
+        <v>128</v>
+      </c>
+      <c r="H82" t="s">
+        <v>33</v>
+      </c>
+      <c r="I82" t="s">
+        <v>70</v>
+      </c>
+      <c r="J82">
+        <v>32</v>
+      </c>
+      <c r="K82">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M82">
+        <v>100</v>
+      </c>
+      <c r="N82">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="O82">
+        <v>0.74</v>
+      </c>
+      <c r="P82">
+        <v>0.9</v>
+      </c>
+      <c r="Q82">
+        <v>5.3019999999999998E-2</v>
+      </c>
+      <c r="R82" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>44</v>
+      </c>
+      <c r="B83">
+        <v>9</v>
+      </c>
+      <c r="F83">
+        <v>128</v>
+      </c>
+      <c r="H83" t="s">
+        <v>33</v>
+      </c>
+      <c r="I83" t="s">
+        <v>70</v>
+      </c>
+      <c r="J83">
+        <v>32</v>
+      </c>
+      <c r="K83">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M83">
+        <v>100</v>
+      </c>
+      <c r="N83">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="O83">
+        <v>0.74</v>
+      </c>
+      <c r="P83">
+        <v>0.9</v>
+      </c>
+      <c r="Q83">
+        <v>5.3019999999999998E-2</v>
+      </c>
+      <c r="R83" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>44</v>
+      </c>
+      <c r="B84">
+        <v>10</v>
+      </c>
+      <c r="F84">
+        <v>128</v>
+      </c>
+      <c r="H84" t="s">
+        <v>33</v>
+      </c>
+      <c r="I84" t="s">
+        <v>70</v>
+      </c>
+      <c r="J84">
+        <v>32</v>
+      </c>
+      <c r="K84">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M84">
+        <v>100</v>
+      </c>
+      <c r="N84">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="O84">
+        <v>0.74</v>
+      </c>
+      <c r="P84">
+        <v>0.9</v>
+      </c>
+      <c r="Q84">
+        <v>5.3019999999999998E-2</v>
+      </c>
+      <c r="R84" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>44</v>
+      </c>
+      <c r="B85">
+        <v>11</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="H85" t="s">
+        <v>69</v>
+      </c>
+      <c r="I85" t="s">
+        <v>70</v>
+      </c>
+      <c r="J85">
+        <v>32</v>
+      </c>
+      <c r="K85">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M85">
+        <v>100</v>
+      </c>
+      <c r="N85">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="O85">
+        <v>0.74</v>
+      </c>
+      <c r="P85">
+        <v>0.9</v>
+      </c>
+      <c r="Q85">
+        <v>5.3019999999999998E-2</v>
+      </c>
+      <c r="R85" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>49</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>512</v>
+      </c>
+      <c r="E86" t="b">
+        <v>0</v>
+      </c>
+      <c r="H86" t="s">
+        <v>27</v>
+      </c>
+      <c r="I86" t="s">
+        <v>70</v>
+      </c>
+      <c r="J86">
+        <v>32</v>
+      </c>
+      <c r="K86">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M86">
+        <v>100</v>
+      </c>
+      <c r="N86">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="O86">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="P86">
+        <v>0.9</v>
+      </c>
+      <c r="Q86">
+        <v>6.59E-2</v>
+      </c>
+      <c r="R86" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>49</v>
+      </c>
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="F87">
+        <v>512</v>
+      </c>
+      <c r="H87" t="s">
+        <v>33</v>
+      </c>
+      <c r="I87" t="s">
+        <v>70</v>
+      </c>
+      <c r="J87">
+        <v>32</v>
+      </c>
+      <c r="K87">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M87">
+        <v>100</v>
+      </c>
+      <c r="N87">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="O87">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="P87">
+        <v>0.9</v>
+      </c>
+      <c r="Q87">
+        <v>6.59E-2</v>
+      </c>
+      <c r="R87" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>49</v>
+      </c>
+      <c r="B88">
+        <v>3</v>
+      </c>
+      <c r="F88">
+        <v>512</v>
+      </c>
+      <c r="H88" t="s">
+        <v>33</v>
+      </c>
+      <c r="I88" t="s">
+        <v>70</v>
+      </c>
+      <c r="J88">
+        <v>32</v>
+      </c>
+      <c r="K88">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M88">
+        <v>100</v>
+      </c>
+      <c r="N88">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="O88">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="P88">
+        <v>0.9</v>
+      </c>
+      <c r="Q88">
+        <v>6.59E-2</v>
+      </c>
+      <c r="R88" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>49</v>
+      </c>
+      <c r="B89">
+        <v>4</v>
+      </c>
+      <c r="F89">
+        <v>256</v>
+      </c>
+      <c r="H89" t="s">
+        <v>33</v>
+      </c>
+      <c r="I89" t="s">
+        <v>70</v>
+      </c>
+      <c r="J89">
+        <v>32</v>
+      </c>
+      <c r="K89">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M89">
+        <v>100</v>
+      </c>
+      <c r="N89">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="O89">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="P89">
+        <v>0.9</v>
+      </c>
+      <c r="Q89">
+        <v>6.59E-2</v>
+      </c>
+      <c r="R89" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>49</v>
+      </c>
+      <c r="B90">
+        <v>5</v>
+      </c>
+      <c r="F90">
+        <v>256</v>
+      </c>
+      <c r="H90" t="s">
+        <v>33</v>
+      </c>
+      <c r="I90" t="s">
+        <v>70</v>
+      </c>
+      <c r="J90">
+        <v>32</v>
+      </c>
+      <c r="K90">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M90">
+        <v>100</v>
+      </c>
+      <c r="N90">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="O90">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="P90">
+        <v>0.9</v>
+      </c>
+      <c r="Q90">
+        <v>6.59E-2</v>
+      </c>
+      <c r="R90" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>49</v>
+      </c>
+      <c r="B91">
+        <v>6</v>
+      </c>
+      <c r="F91">
+        <v>256</v>
+      </c>
+      <c r="H91" t="s">
+        <v>33</v>
+      </c>
+      <c r="I91" t="s">
+        <v>70</v>
+      </c>
+      <c r="J91">
+        <v>32</v>
+      </c>
+      <c r="K91">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M91">
+        <v>100</v>
+      </c>
+      <c r="N91">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="O91">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="P91">
+        <v>0.9</v>
+      </c>
+      <c r="Q91">
+        <v>6.59E-2</v>
+      </c>
+      <c r="R91" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>49</v>
+      </c>
+      <c r="B92">
+        <v>7</v>
+      </c>
+      <c r="F92">
+        <v>128</v>
+      </c>
+      <c r="H92" t="s">
+        <v>33</v>
+      </c>
+      <c r="I92" t="s">
+        <v>70</v>
+      </c>
+      <c r="J92">
+        <v>32</v>
+      </c>
+      <c r="K92">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M92">
+        <v>100</v>
+      </c>
+      <c r="N92">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="O92">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="P92">
+        <v>0.9</v>
+      </c>
+      <c r="Q92">
+        <v>6.59E-2</v>
+      </c>
+      <c r="R92" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>49</v>
+      </c>
+      <c r="B93">
+        <v>8</v>
+      </c>
+      <c r="F93">
+        <v>128</v>
+      </c>
+      <c r="H93" t="s">
+        <v>33</v>
+      </c>
+      <c r="I93" t="s">
+        <v>70</v>
+      </c>
+      <c r="J93">
+        <v>32</v>
+      </c>
+      <c r="K93">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M93">
+        <v>100</v>
+      </c>
+      <c r="N93">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="O93">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="P93">
+        <v>0.9</v>
+      </c>
+      <c r="Q93">
+        <v>6.59E-2</v>
+      </c>
+      <c r="R93" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>49</v>
+      </c>
+      <c r="B94">
+        <v>9</v>
+      </c>
+      <c r="F94">
+        <v>64</v>
+      </c>
+      <c r="H94" t="s">
+        <v>33</v>
+      </c>
+      <c r="I94" t="s">
+        <v>70</v>
+      </c>
+      <c r="J94">
+        <v>32</v>
+      </c>
+      <c r="K94">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M94">
+        <v>100</v>
+      </c>
+      <c r="N94">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="O94">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="P94">
+        <v>0.9</v>
+      </c>
+      <c r="Q94">
+        <v>6.59E-2</v>
+      </c>
+      <c r="R94" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>49</v>
+      </c>
+      <c r="B95">
+        <v>10</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
+      </c>
+      <c r="H95" t="s">
+        <v>69</v>
+      </c>
+      <c r="I95" t="s">
+        <v>70</v>
+      </c>
+      <c r="J95">
+        <v>32</v>
+      </c>
+      <c r="K95">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M95">
+        <v>100</v>
+      </c>
+      <c r="N95">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="O95">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="P95">
+        <v>0.9</v>
+      </c>
+      <c r="Q95">
+        <v>6.59E-2</v>
+      </c>
+      <c r="R95" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Trying to get these plots right
</commit_message>
<xml_diff>
--- a/NEW/statistical_analysis/Networks Compared.xlsx
+++ b/NEW/statistical_analysis/Networks Compared.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerhard\Documents\MSc-thesis\NEW\statistical_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95ED5591-A72C-4D4C-951C-22EAE7839BA0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0F90DA-88E6-4291-BB1F-6315A309FEEE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="-120" windowWidth="27300" windowHeight="16440" xr2:uid="{42FDFE43-F33F-4893-BA97-B5C32084F215}"/>
+    <workbookView xWindow="1620" yWindow="-120" windowWidth="27300" windowHeight="16440" activeTab="3" xr2:uid="{42FDFE43-F33F-4893-BA97-B5C32084F215}"/>
   </bookViews>
   <sheets>
     <sheet name="Fully conected" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="CNN (Conv1D)" sheetId="3" r:id="rId3"/>
     <sheet name="LSTM" sheetId="4" r:id="rId4"/>
     <sheet name="XGBoost" sheetId="5" r:id="rId5"/>
+    <sheet name="Merged Ensemble" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2707" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2731" uniqueCount="119">
   <si>
     <t>Model Number</t>
   </si>
@@ -389,6 +390,9 @@
   </si>
   <si>
     <t>Column Sums, Mean Pixel Value, Standard deviation pixel value,l2 norm of image, max pixel value, 6 timebins summed sequentially, lagged differences of 6-column sums with lag=1, Chamber Gain Corrected, tracks that have 6 tracklets, all electrons and an equal number of pions, scaled as follows: x=x/max(x)</t>
+  </si>
+  <si>
+    <t>still need to fill this in if I get the energy from somewhere</t>
   </si>
 </sst>
 </file>
@@ -766,7 +770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32EF017-127E-4272-A45C-8B2FC1D130CC}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
@@ -1502,9 +1506,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D847C349-F495-423A-9F1C-FAD29C38B92F}">
   <dimension ref="A1:W372"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A354" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W370" sqref="W370"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A345" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L371" sqref="L371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18916,8 +18920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4356D11A-C020-4F7F-859E-F8F25B3322AC}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
@@ -21119,8 +21123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26382EEA-56AD-452C-9D78-7AC7571B137C}">
   <dimension ref="A1:R95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="D95" sqref="D95"/>
     </sheetView>
@@ -25273,7 +25277,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25349,4 +25353,119 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4635CD4A-899F-4AED-947F-4E1299E91F38}">
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Moving chapters and sections around to give myself some peace of mind
</commit_message>
<xml_diff>
--- a/NEW/statistical_analysis/Networks Compared.xlsx
+++ b/NEW/statistical_analysis/Networks Compared.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerhard\Documents\MSc-thesis\NEW\statistical_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0F90DA-88E6-4291-BB1F-6315A309FEEE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB859C21-AB00-443D-A12D-B31F314B3E94}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="-120" windowWidth="27300" windowHeight="16440" activeTab="3" xr2:uid="{42FDFE43-F33F-4893-BA97-B5C32084F215}"/>
+    <workbookView xWindow="1620" yWindow="-120" windowWidth="27300" windowHeight="16440" activeTab="1" xr2:uid="{42FDFE43-F33F-4893-BA97-B5C32084F215}"/>
   </bookViews>
   <sheets>
     <sheet name="Fully conected" sheetId="1" r:id="rId1"/>
@@ -1506,9 +1506,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D847C349-F495-423A-9F1C-FAD29C38B92F}">
   <dimension ref="A1:W372"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A345" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L371" sqref="L371"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V157" sqref="V157:V160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8619,7 +8619,7 @@
         <v>0.9</v>
       </c>
       <c r="V157">
-        <v>0.02</v>
+        <v>2.98E-2</v>
       </c>
       <c r="W157" t="s">
         <v>71</v>
@@ -8669,7 +8669,7 @@
         <v>0.9</v>
       </c>
       <c r="V158">
-        <v>0.02</v>
+        <v>2.98E-2</v>
       </c>
       <c r="W158" t="s">
         <v>71</v>
@@ -8713,7 +8713,7 @@
         <v>0.9</v>
       </c>
       <c r="V159">
-        <v>0.02</v>
+        <v>2.98E-2</v>
       </c>
       <c r="W159" t="s">
         <v>71</v>
@@ -8760,7 +8760,7 @@
         <v>0.9</v>
       </c>
       <c r="V160">
-        <v>0.02</v>
+        <v>2.98E-2</v>
       </c>
       <c r="W160" t="s">
         <v>71</v>
@@ -21123,7 +21123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26382EEA-56AD-452C-9D78-7AC7571B137C}">
   <dimension ref="A1:R95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="D95" sqref="D95"/>

</xml_diff>

<commit_message>
Reset soft head to remove large files
</commit_message>
<xml_diff>
--- a/NEW/statistical_analysis/Networks Compared.xlsx
+++ b/NEW/statistical_analysis/Networks Compared.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerhard\Documents\MSc-thesis\NEW\statistical_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3F491E-F01C-4A13-B03A-203C17872F88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA400D67-C39F-4430-9A59-1D2C7A1720A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="-120" windowWidth="27300" windowHeight="16440" activeTab="1" xr2:uid="{42FDFE43-F33F-4893-BA97-B5C32084F215}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2299" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2304" uniqueCount="123">
   <si>
     <t>Model Number</t>
   </si>
@@ -390,6 +390,21 @@
   </si>
   <si>
     <t>still need to fill this in if I get the energy from somewhere</t>
+  </si>
+  <si>
+    <t>M53</t>
+  </si>
+  <si>
+    <t>nPions</t>
+  </si>
+  <si>
+    <t>nElectrons</t>
+  </si>
+  <si>
+    <t>Scaling Strategy</t>
+  </si>
+  <si>
+    <t>P range</t>
   </si>
 </sst>
 </file>
@@ -1501,11 +1516,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D847C349-F495-423A-9F1C-FAD29C38B92F}">
-  <dimension ref="A1:W289"/>
+  <dimension ref="A1:AA290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A268" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J281" sqref="J281"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,10 +1546,14 @@
     <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.85546875" customWidth="1"/>
+    <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.28515625" customWidth="1"/>
+    <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1602,10 +1621,22 @@
         <v>10</v>
       </c>
       <c r="W1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="X1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1651,11 +1682,11 @@
       <c r="V2">
         <v>0.6</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AA2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1707,11 +1738,11 @@
       <c r="V3">
         <v>0.6</v>
       </c>
-      <c r="W3" t="s">
+      <c r="AA3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1754,11 +1785,11 @@
       <c r="V4">
         <v>0.6</v>
       </c>
-      <c r="W4" t="s">
+      <c r="AA4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1801,11 +1832,11 @@
       <c r="V5">
         <v>0.6</v>
       </c>
-      <c r="W5" t="s">
+      <c r="AA5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1851,11 +1882,11 @@
       <c r="V6">
         <v>0.54</v>
       </c>
-      <c r="W6" t="s">
+      <c r="AA6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1907,11 +1938,11 @@
       <c r="V7">
         <v>0.54</v>
       </c>
-      <c r="W7" t="s">
+      <c r="AA7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1954,11 +1985,11 @@
       <c r="V8">
         <v>0.54</v>
       </c>
-      <c r="W8" t="s">
+      <c r="AA8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2001,11 +2032,11 @@
       <c r="V9">
         <v>0.54</v>
       </c>
-      <c r="W9" t="s">
+      <c r="AA9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2051,11 +2082,11 @@
       <c r="V10">
         <v>0.75900000000000001</v>
       </c>
-      <c r="W10" t="s">
+      <c r="AA10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -2101,11 +2132,11 @@
       <c r="V11">
         <v>0.75900000000000001</v>
       </c>
-      <c r="W11" t="s">
+      <c r="AA11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2157,11 +2188,11 @@
       <c r="V12">
         <v>0.75900000000000001</v>
       </c>
-      <c r="W12" t="s">
+      <c r="AA12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2204,11 +2235,11 @@
       <c r="V13">
         <v>0.75900000000000001</v>
       </c>
-      <c r="W13" t="s">
+      <c r="AA13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2251,11 +2282,11 @@
       <c r="V14">
         <v>0.75900000000000001</v>
       </c>
-      <c r="W14" t="s">
+      <c r="AA14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2298,11 +2329,11 @@
       <c r="V15">
         <v>0.75900000000000001</v>
       </c>
-      <c r="W15" t="s">
+      <c r="AA15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -2345,11 +2376,11 @@
       <c r="V16">
         <v>0.75900000000000001</v>
       </c>
-      <c r="W16" t="s">
+      <c r="AA16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2395,11 +2426,11 @@
       <c r="V17">
         <v>0.89</v>
       </c>
-      <c r="W17" t="s">
+      <c r="AA17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -2448,11 +2479,11 @@
       <c r="V18">
         <v>0.89</v>
       </c>
-      <c r="W18" t="s">
+      <c r="AA18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -2492,11 +2523,11 @@
       <c r="V19">
         <v>0.89</v>
       </c>
-      <c r="W19" t="s">
+      <c r="AA19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2536,11 +2567,11 @@
       <c r="V20">
         <v>0.89</v>
       </c>
-      <c r="W20" t="s">
+      <c r="AA20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2580,11 +2611,11 @@
       <c r="V21">
         <v>0.89</v>
       </c>
-      <c r="W21" t="s">
+      <c r="AA21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -2624,11 +2655,11 @@
       <c r="V22">
         <v>0.89</v>
       </c>
-      <c r="W22" t="s">
+      <c r="AA22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -2668,11 +2699,11 @@
       <c r="V23">
         <v>0.89</v>
       </c>
-      <c r="W23" t="s">
+      <c r="AA23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -2712,11 +2743,11 @@
       <c r="V24">
         <v>0.89</v>
       </c>
-      <c r="W24" t="s">
+      <c r="AA24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -2756,11 +2787,11 @@
       <c r="V25">
         <v>0.89</v>
       </c>
-      <c r="W25" t="s">
+      <c r="AA25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -2800,11 +2831,11 @@
       <c r="V26">
         <v>0.89</v>
       </c>
-      <c r="W26" t="s">
+      <c r="AA26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -2844,11 +2875,11 @@
       <c r="V27">
         <v>0.89</v>
       </c>
-      <c r="W27" t="s">
+      <c r="AA27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -2888,11 +2919,11 @@
       <c r="V28">
         <v>0.89</v>
       </c>
-      <c r="W28" t="s">
+      <c r="AA28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -2935,11 +2966,11 @@
       <c r="V29">
         <v>0.89</v>
       </c>
-      <c r="W29" t="s">
+      <c r="AA29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -2985,11 +3016,11 @@
       <c r="V30">
         <v>0.9</v>
       </c>
-      <c r="W30" t="s">
+      <c r="AA30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -3038,11 +3069,11 @@
       <c r="V31">
         <v>0.9</v>
       </c>
-      <c r="W31" t="s">
+      <c r="AA31" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -3082,11 +3113,11 @@
       <c r="V32">
         <v>0.9</v>
       </c>
-      <c r="W32" t="s">
+      <c r="AA32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -3126,11 +3157,11 @@
       <c r="V33">
         <v>0.9</v>
       </c>
-      <c r="W33" t="s">
+      <c r="AA33" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -3170,11 +3201,11 @@
       <c r="V34">
         <v>0.9</v>
       </c>
-      <c r="W34" t="s">
+      <c r="AA34" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -3214,11 +3245,11 @@
       <c r="V35">
         <v>0.9</v>
       </c>
-      <c r="W35" t="s">
+      <c r="AA35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -3258,11 +3289,11 @@
       <c r="V36">
         <v>0.9</v>
       </c>
-      <c r="W36" t="s">
+      <c r="AA36" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -3302,11 +3333,11 @@
       <c r="V37">
         <v>0.9</v>
       </c>
-      <c r="W37" t="s">
+      <c r="AA37" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -3346,11 +3377,11 @@
       <c r="V38">
         <v>0.9</v>
       </c>
-      <c r="W38" t="s">
+      <c r="AA38" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -3390,11 +3421,11 @@
       <c r="V39">
         <v>0.9</v>
       </c>
-      <c r="W39" t="s">
+      <c r="AA39" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -3434,11 +3465,11 @@
       <c r="V40">
         <v>0.9</v>
       </c>
-      <c r="W40" t="s">
+      <c r="AA40" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -3478,11 +3509,11 @@
       <c r="V41">
         <v>0.9</v>
       </c>
-      <c r="W41" t="s">
+      <c r="AA41" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -3522,11 +3553,11 @@
       <c r="V42">
         <v>0.9</v>
       </c>
-      <c r="W42" t="s">
+      <c r="AA42" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -3566,11 +3597,11 @@
       <c r="V43">
         <v>0.9</v>
       </c>
-      <c r="W43" t="s">
+      <c r="AA43" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -3610,11 +3641,11 @@
       <c r="V44">
         <v>0.9</v>
       </c>
-      <c r="W44" t="s">
+      <c r="AA44" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -3654,11 +3685,11 @@
       <c r="V45">
         <v>0.9</v>
       </c>
-      <c r="W45" t="s">
+      <c r="AA45" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -3701,11 +3732,11 @@
       <c r="V46">
         <v>0.9</v>
       </c>
-      <c r="W46" t="s">
+      <c r="AA46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -3757,11 +3788,11 @@
       <c r="V47">
         <v>0.88</v>
       </c>
-      <c r="W47" t="s">
+      <c r="AA47" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -3813,11 +3844,11 @@
       <c r="V48">
         <v>0.88</v>
       </c>
-      <c r="W48" t="s">
+      <c r="AA48" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -3866,11 +3897,11 @@
       <c r="V49">
         <v>0.88</v>
       </c>
-      <c r="W49" t="s">
+      <c r="AA49" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -3913,11 +3944,11 @@
       <c r="V50">
         <v>0.88</v>
       </c>
-      <c r="W50" t="s">
+      <c r="AA50" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -3960,11 +3991,11 @@
       <c r="V51">
         <v>0.88</v>
       </c>
-      <c r="W51" t="s">
+      <c r="AA51" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -4007,11 +4038,11 @@
       <c r="V52">
         <v>0.88</v>
       </c>
-      <c r="W52" t="s">
+      <c r="AA52" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -4054,11 +4085,11 @@
       <c r="V53">
         <v>0.88</v>
       </c>
-      <c r="W53" t="s">
+      <c r="AA53" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -4101,11 +4132,11 @@
       <c r="V54">
         <v>0.88</v>
       </c>
-      <c r="W54" t="s">
+      <c r="AA54" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -4151,11 +4182,11 @@
       <c r="V55">
         <v>0.88</v>
       </c>
-      <c r="W55" t="s">
+      <c r="AA55" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -4207,11 +4238,11 @@
       <c r="V56">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W56" t="s">
+      <c r="AA56" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -4263,11 +4294,11 @@
       <c r="V57">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W57" t="s">
+      <c r="AA57" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -4310,11 +4341,11 @@
       <c r="V58">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W58" t="s">
+      <c r="AA58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -4357,11 +4388,11 @@
       <c r="V59">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W59" t="s">
+      <c r="AA59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -4404,11 +4435,11 @@
       <c r="V60">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W60" t="s">
+      <c r="AA60" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -4451,11 +4482,11 @@
       <c r="V61">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W61" t="s">
+      <c r="AA61" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -4498,11 +4529,11 @@
       <c r="V62">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W62" t="s">
+      <c r="AA62" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>58</v>
       </c>
@@ -4545,11 +4576,11 @@
       <c r="V63">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W63" t="s">
+      <c r="AA63" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>58</v>
       </c>
@@ -4592,11 +4623,11 @@
       <c r="V64">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W64" t="s">
+      <c r="AA64" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>58</v>
       </c>
@@ -4639,11 +4670,11 @@
       <c r="V65">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W65" t="s">
+      <c r="AA65" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>58</v>
       </c>
@@ -4686,11 +4717,11 @@
       <c r="V66">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W66" t="s">
+      <c r="AA66" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>58</v>
       </c>
@@ -4733,11 +4764,11 @@
       <c r="V67">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W67" t="s">
+      <c r="AA67" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>58</v>
       </c>
@@ -4780,11 +4811,11 @@
       <c r="V68">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W68" t="s">
+      <c r="AA68" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>58</v>
       </c>
@@ -4827,11 +4858,11 @@
       <c r="V69">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W69" t="s">
+      <c r="AA69" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>58</v>
       </c>
@@ -4877,11 +4908,11 @@
       <c r="V70">
         <v>0.88200000000000001</v>
       </c>
-      <c r="W70" t="s">
+      <c r="AA70" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>59</v>
       </c>
@@ -4927,11 +4958,11 @@
       <c r="V71">
         <v>0.06</v>
       </c>
-      <c r="W71" t="s">
+      <c r="AA71" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>59</v>
       </c>
@@ -4971,11 +5002,11 @@
       <c r="V72">
         <v>0.06</v>
       </c>
-      <c r="W72" t="s">
+      <c r="AA72" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>59</v>
       </c>
@@ -5018,11 +5049,11 @@
       <c r="V73">
         <v>0.06</v>
       </c>
-      <c r="W73" t="s">
+      <c r="AA73" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>60</v>
       </c>
@@ -5068,11 +5099,11 @@
       <c r="V74">
         <v>2.98E-2</v>
       </c>
-      <c r="W74" t="s">
+      <c r="AA74" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>60</v>
       </c>
@@ -5118,11 +5149,11 @@
       <c r="V75">
         <v>2.98E-2</v>
       </c>
-      <c r="W75" t="s">
+      <c r="AA75" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>60</v>
       </c>
@@ -5162,11 +5193,11 @@
       <c r="V76">
         <v>2.98E-2</v>
       </c>
-      <c r="W76" t="s">
+      <c r="AA76" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>60</v>
       </c>
@@ -5209,11 +5240,11 @@
       <c r="V77">
         <v>2.98E-2</v>
       </c>
-      <c r="W77" t="s">
+      <c r="AA77" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>61</v>
       </c>
@@ -5259,11 +5290,11 @@
       <c r="V78">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="W78" t="s">
+      <c r="AA78" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>61</v>
       </c>
@@ -5303,11 +5334,11 @@
       <c r="V79">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="W79" t="s">
+      <c r="AA79" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>61</v>
       </c>
@@ -5347,11 +5378,11 @@
       <c r="V80">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="W80" t="s">
+      <c r="AA80" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>61</v>
       </c>
@@ -5391,11 +5422,11 @@
       <c r="V81">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="W81" t="s">
+      <c r="AA81" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>61</v>
       </c>
@@ -5435,11 +5466,11 @@
       <c r="V82">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="W82" t="s">
+      <c r="AA82" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>61</v>
       </c>
@@ -5482,11 +5513,11 @@
       <c r="V83">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="W83" t="s">
+      <c r="AA83" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>62</v>
       </c>
@@ -5532,11 +5563,11 @@
       <c r="V84">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="W84" t="s">
+      <c r="AA84" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>62</v>
       </c>
@@ -5582,11 +5613,11 @@
       <c r="V85">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="W85" t="s">
+      <c r="AA85" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>62</v>
       </c>
@@ -5632,11 +5663,11 @@
       <c r="V86">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="W86" t="s">
+      <c r="AA86" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>62</v>
       </c>
@@ -5682,11 +5713,11 @@
       <c r="V87">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="W87" t="s">
+      <c r="AA87" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>62</v>
       </c>
@@ -5726,11 +5757,11 @@
       <c r="V88">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="W88" t="s">
+      <c r="AA88" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>62</v>
       </c>
@@ -5770,11 +5801,11 @@
       <c r="V89">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="W89" t="s">
+      <c r="AA89" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>62</v>
       </c>
@@ -5814,11 +5845,11 @@
       <c r="V90">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="W90" t="s">
+      <c r="AA90" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>62</v>
       </c>
@@ -5858,11 +5889,11 @@
       <c r="V91">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="W91" t="s">
+      <c r="AA91" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>62</v>
       </c>
@@ -5905,11 +5936,11 @@
       <c r="V92">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="W92" t="s">
+      <c r="AA92" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>63</v>
       </c>
@@ -5958,11 +5989,11 @@
       <c r="V93">
         <v>5.5599999999999997E-2</v>
       </c>
-      <c r="W93" t="s">
+      <c r="AA93" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>63</v>
       </c>
@@ -6011,11 +6042,11 @@
       <c r="V94">
         <v>5.5599999999999997E-2</v>
       </c>
-      <c r="W94" t="s">
+      <c r="AA94" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>63</v>
       </c>
@@ -6061,11 +6092,11 @@
       <c r="V95">
         <v>5.5599999999999997E-2</v>
       </c>
-      <c r="W95" t="s">
+      <c r="AA95" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>63</v>
       </c>
@@ -6105,11 +6136,11 @@
       <c r="V96">
         <v>5.5599999999999997E-2</v>
       </c>
-      <c r="W96" t="s">
+      <c r="AA96" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>63</v>
       </c>
@@ -6149,11 +6180,11 @@
       <c r="V97">
         <v>5.5599999999999997E-2</v>
       </c>
-      <c r="W97" t="s">
+      <c r="AA97" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>63</v>
       </c>
@@ -6193,11 +6224,11 @@
       <c r="V98">
         <v>5.5599999999999997E-2</v>
       </c>
-      <c r="W98" t="s">
+      <c r="AA98" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>63</v>
       </c>
@@ -6240,11 +6271,11 @@
       <c r="V99">
         <v>5.5599999999999997E-2</v>
       </c>
-      <c r="W99" t="s">
+      <c r="AA99" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>64</v>
       </c>
@@ -6290,11 +6321,11 @@
       <c r="V100">
         <v>0.255</v>
       </c>
-      <c r="W100" t="s">
+      <c r="AA100" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>64</v>
       </c>
@@ -6337,11 +6368,11 @@
       <c r="V101">
         <v>0.255</v>
       </c>
-      <c r="W101" t="s">
+      <c r="AA101" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>64</v>
       </c>
@@ -6384,11 +6415,11 @@
       <c r="V102">
         <v>0.255</v>
       </c>
-      <c r="W102" t="s">
+      <c r="AA102" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>65</v>
       </c>
@@ -6434,11 +6465,11 @@
       <c r="V103">
         <v>0.157</v>
       </c>
-      <c r="W103" t="s">
+      <c r="AA103" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>65</v>
       </c>
@@ -6481,11 +6512,11 @@
       <c r="V104">
         <v>0.157</v>
       </c>
-      <c r="W104" t="s">
+      <c r="AA104" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>65</v>
       </c>
@@ -6528,11 +6559,11 @@
       <c r="V105">
         <v>0.157</v>
       </c>
-      <c r="W105" t="s">
+      <c r="AA105" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>65</v>
       </c>
@@ -6575,11 +6606,11 @@
       <c r="V106">
         <v>0.157</v>
       </c>
-      <c r="W106" t="s">
+      <c r="AA106" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>66</v>
       </c>
@@ -6625,11 +6656,11 @@
       <c r="V107">
         <v>0.16300000000000001</v>
       </c>
-      <c r="W107" t="s">
+      <c r="AA107" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>66</v>
       </c>
@@ -6672,11 +6703,11 @@
       <c r="V108">
         <v>0.16300000000000001</v>
       </c>
-      <c r="W108" t="s">
+      <c r="AA108" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>66</v>
       </c>
@@ -6719,11 +6750,11 @@
       <c r="V109">
         <v>0.16300000000000001</v>
       </c>
-      <c r="W109" t="s">
+      <c r="AA109" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>66</v>
       </c>
@@ -6766,11 +6797,11 @@
       <c r="V110">
         <v>0.16300000000000001</v>
       </c>
-      <c r="W110" t="s">
+      <c r="AA110" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>66</v>
       </c>
@@ -6813,11 +6844,11 @@
       <c r="V111">
         <v>0.16300000000000001</v>
       </c>
-      <c r="W111" t="s">
+      <c r="AA111" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>67</v>
       </c>
@@ -6863,11 +6894,11 @@
       <c r="V112">
         <v>0.13400000000000001</v>
       </c>
-      <c r="W112" t="s">
+      <c r="AA112" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>67</v>
       </c>
@@ -6910,11 +6941,11 @@
       <c r="V113">
         <v>0.13400000000000001</v>
       </c>
-      <c r="W113" t="s">
+      <c r="AA113" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>67</v>
       </c>
@@ -6957,11 +6988,11 @@
       <c r="V114">
         <v>0.13400000000000001</v>
       </c>
-      <c r="W114" t="s">
+      <c r="AA114" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>67</v>
       </c>
@@ -7004,11 +7035,11 @@
       <c r="V115">
         <v>0.13400000000000001</v>
       </c>
-      <c r="W115" t="s">
+      <c r="AA115" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>67</v>
       </c>
@@ -7051,11 +7082,11 @@
       <c r="V116">
         <v>0.13400000000000001</v>
       </c>
-      <c r="W116" t="s">
+      <c r="AA116" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>81</v>
       </c>
@@ -7101,11 +7132,11 @@
       <c r="V117">
         <v>0.112</v>
       </c>
-      <c r="W117" t="s">
+      <c r="AA117" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>81</v>
       </c>
@@ -7148,11 +7179,11 @@
       <c r="V118">
         <v>0.112</v>
       </c>
-      <c r="W118" t="s">
+      <c r="AA118" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>81</v>
       </c>
@@ -7195,11 +7226,11 @@
       <c r="V119">
         <v>0.112</v>
       </c>
-      <c r="W119" t="s">
+      <c r="AA119" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>82</v>
       </c>
@@ -7245,11 +7276,11 @@
       <c r="V120">
         <v>8.5599999999999996E-2</v>
       </c>
-      <c r="W120" t="s">
+      <c r="AA120" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>82</v>
       </c>
@@ -7292,11 +7323,11 @@
       <c r="V121">
         <v>8.5599999999999996E-2</v>
       </c>
-      <c r="W121" t="s">
+      <c r="AA121" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>82</v>
       </c>
@@ -7339,11 +7370,11 @@
       <c r="V122">
         <v>8.5599999999999996E-2</v>
       </c>
-      <c r="W122" t="s">
+      <c r="AA122" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>82</v>
       </c>
@@ -7386,11 +7417,11 @@
       <c r="V123">
         <v>8.5599999999999996E-2</v>
       </c>
-      <c r="W123" t="s">
+      <c r="AA123" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>83</v>
       </c>
@@ -7430,11 +7461,11 @@
       <c r="V124">
         <v>0.4178</v>
       </c>
-      <c r="W124" t="s">
+      <c r="AA124" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>83</v>
       </c>
@@ -7480,11 +7511,11 @@
       <c r="V125">
         <v>0.4178</v>
       </c>
-      <c r="W125" t="s">
+      <c r="AA125" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>83</v>
       </c>
@@ -7533,11 +7564,11 @@
       <c r="V126">
         <v>0.4178</v>
       </c>
-      <c r="W126" t="s">
+      <c r="AA126" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>83</v>
       </c>
@@ -7580,11 +7611,11 @@
       <c r="V127">
         <v>0.4178</v>
       </c>
-      <c r="W127" t="s">
+      <c r="AA127" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>83</v>
       </c>
@@ -7627,11 +7658,11 @@
       <c r="V128">
         <v>0.4178</v>
       </c>
-      <c r="W128" t="s">
+      <c r="AA128" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>83</v>
       </c>
@@ -7674,11 +7705,11 @@
       <c r="V129">
         <v>0.4178</v>
       </c>
-      <c r="W129" t="s">
+      <c r="AA129" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>85</v>
       </c>
@@ -7724,11 +7755,11 @@
       <c r="V130">
         <v>0.1003</v>
       </c>
-      <c r="W130" t="s">
+      <c r="AA130" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>85</v>
       </c>
@@ -7777,11 +7808,11 @@
       <c r="V131">
         <v>0.1003</v>
       </c>
-      <c r="W131" t="s">
+      <c r="AA131" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>85</v>
       </c>
@@ -7824,11 +7855,11 @@
       <c r="V132">
         <v>0.1003</v>
       </c>
-      <c r="W132" t="s">
+      <c r="AA132" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>85</v>
       </c>
@@ -7871,11 +7902,11 @@
       <c r="V133">
         <v>0.1003</v>
       </c>
-      <c r="W133" t="s">
+      <c r="AA133" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>85</v>
       </c>
@@ -7918,11 +7949,11 @@
       <c r="V134">
         <v>0.1003</v>
       </c>
-      <c r="W134" t="s">
+      <c r="AA134" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>85</v>
       </c>
@@ -7965,11 +7996,11 @@
       <c r="V135">
         <v>0.1003</v>
       </c>
-      <c r="W135" t="s">
+      <c r="AA135" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>86</v>
       </c>
@@ -8009,11 +8040,11 @@
       <c r="V136">
         <v>0.48849999999999999</v>
       </c>
-      <c r="W136" t="s">
+      <c r="AA136" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>86</v>
       </c>
@@ -8059,11 +8090,11 @@
       <c r="V137">
         <v>0.48849999999999999</v>
       </c>
-      <c r="W137" t="s">
+      <c r="AA137" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>86</v>
       </c>
@@ -8106,11 +8137,11 @@
       <c r="V138">
         <v>0.48849999999999999</v>
       </c>
-      <c r="W138" t="s">
+      <c r="AA138" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>86</v>
       </c>
@@ -8153,11 +8184,11 @@
       <c r="V139">
         <v>0.48849999999999999</v>
       </c>
-      <c r="W139" t="s">
+      <c r="AA139" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>87</v>
       </c>
@@ -8197,11 +8228,11 @@
       <c r="V140">
         <v>0.47399999999999998</v>
       </c>
-      <c r="W140" t="s">
+      <c r="AA140" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>87</v>
       </c>
@@ -8247,11 +8278,11 @@
       <c r="V141">
         <v>0.47399999999999998</v>
       </c>
-      <c r="W141" t="s">
+      <c r="AA141" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>87</v>
       </c>
@@ -8291,11 +8322,11 @@
       <c r="V142">
         <v>0.47399999999999998</v>
       </c>
-      <c r="W142" t="s">
+      <c r="AA142" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>87</v>
       </c>
@@ -8338,11 +8369,11 @@
       <c r="V143">
         <v>0.47399999999999998</v>
       </c>
-      <c r="W143" t="s">
+      <c r="AA143" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I144">
         <v>0.2</v>
       </c>
@@ -8382,11 +8413,11 @@
       <c r="V144">
         <v>0.47399999999999998</v>
       </c>
-      <c r="W144" t="s">
+      <c r="AA144" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>88</v>
       </c>
@@ -8426,11 +8457,11 @@
       <c r="V145">
         <v>0.46289999999999998</v>
       </c>
-      <c r="W145" t="s">
+      <c r="AA145" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>88</v>
       </c>
@@ -8476,11 +8507,11 @@
       <c r="V146">
         <v>0.46289999999999998</v>
       </c>
-      <c r="W146" t="s">
+      <c r="AA146" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>88</v>
       </c>
@@ -8523,11 +8554,11 @@
       <c r="V147">
         <v>0.46289999999999998</v>
       </c>
-      <c r="W147" t="s">
+      <c r="AA147" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>88</v>
       </c>
@@ -8570,11 +8601,11 @@
       <c r="V148">
         <v>0.46289999999999998</v>
       </c>
-      <c r="W148" t="s">
+      <c r="AA148" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>88</v>
       </c>
@@ -8617,11 +8648,11 @@
       <c r="V149">
         <v>0.46289999999999998</v>
       </c>
-      <c r="W149" t="s">
+      <c r="AA149" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>88</v>
       </c>
@@ -8664,11 +8695,11 @@
       <c r="V150">
         <v>0.46289999999999998</v>
       </c>
-      <c r="W150" t="s">
+      <c r="AA150" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>89</v>
       </c>
@@ -8708,11 +8739,11 @@
       <c r="V151">
         <v>0.31900000000000001</v>
       </c>
-      <c r="W151" t="s">
+      <c r="AA151" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>89</v>
       </c>
@@ -8758,11 +8789,11 @@
       <c r="V152">
         <v>0.31900000000000001</v>
       </c>
-      <c r="W152" t="s">
+      <c r="AA152" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>89</v>
       </c>
@@ -8811,11 +8842,11 @@
       <c r="V153">
         <v>0.31900000000000001</v>
       </c>
-      <c r="W153" t="s">
+      <c r="AA153" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>89</v>
       </c>
@@ -8855,11 +8886,11 @@
       <c r="V154">
         <v>0.31900000000000001</v>
       </c>
-      <c r="W154" t="s">
+      <c r="AA154" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>89</v>
       </c>
@@ -8899,11 +8930,11 @@
       <c r="V155">
         <v>0.31900000000000001</v>
       </c>
-      <c r="W155" t="s">
+      <c r="AA155" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>89</v>
       </c>
@@ -8943,11 +8974,11 @@
       <c r="V156">
         <v>0.31900000000000001</v>
       </c>
-      <c r="W156" t="s">
+      <c r="AA156" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>89</v>
       </c>
@@ -8990,11 +9021,11 @@
       <c r="V157">
         <v>0.31900000000000001</v>
       </c>
-      <c r="W157" t="s">
+      <c r="AA157" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>90</v>
       </c>
@@ -9040,11 +9071,11 @@
       <c r="V158">
         <v>8.6900000000000005E-2</v>
       </c>
-      <c r="W158" t="s">
+      <c r="AA158" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>90</v>
       </c>
@@ -9093,11 +9124,11 @@
       <c r="V159">
         <v>8.6900000000000005E-2</v>
       </c>
-      <c r="W159" t="s">
+      <c r="AA159" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>90</v>
       </c>
@@ -9143,11 +9174,11 @@
       <c r="V160">
         <v>8.6900000000000005E-2</v>
       </c>
-      <c r="W160" t="s">
+      <c r="AA160" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>90</v>
       </c>
@@ -9190,11 +9221,11 @@
       <c r="V161">
         <v>8.6900000000000005E-2</v>
       </c>
-      <c r="W161" t="s">
+      <c r="AA161" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>90</v>
       </c>
@@ -9237,11 +9268,11 @@
       <c r="V162">
         <v>8.6900000000000005E-2</v>
       </c>
-      <c r="W162" t="s">
+      <c r="AA162" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>92</v>
       </c>
@@ -9287,11 +9318,11 @@
       <c r="V163">
         <v>5.7099999999999998E-2</v>
       </c>
-      <c r="W163" t="s">
+      <c r="AA163" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>92</v>
       </c>
@@ -9334,11 +9365,11 @@
       <c r="V164">
         <v>5.7099999999999998E-2</v>
       </c>
-      <c r="W164" t="s">
+      <c r="AA164" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>92</v>
       </c>
@@ -9381,11 +9412,11 @@
       <c r="V165">
         <v>5.7099999999999998E-2</v>
       </c>
-      <c r="W165" t="s">
+      <c r="AA165" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>92</v>
       </c>
@@ -9428,11 +9459,11 @@
       <c r="V166">
         <v>5.7099999999999998E-2</v>
       </c>
-      <c r="W166" t="s">
+      <c r="AA166" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>93</v>
       </c>
@@ -9478,11 +9509,11 @@
       <c r="V167">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="W167" t="s">
+      <c r="AA167" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>93</v>
       </c>
@@ -9525,11 +9556,11 @@
       <c r="V168">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="W168" t="s">
+      <c r="AA168" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>93</v>
       </c>
@@ -9572,11 +9603,11 @@
       <c r="V169">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="W169" t="s">
+      <c r="AA169" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>93</v>
       </c>
@@ -9619,11 +9650,11 @@
       <c r="V170">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="W170" t="s">
+      <c r="AA170" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>93</v>
       </c>
@@ -9666,11 +9697,11 @@
       <c r="V171">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="W171" t="s">
+      <c r="AA171" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="172" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>93</v>
       </c>
@@ -9713,11 +9744,11 @@
       <c r="V172">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="W172" t="s">
+      <c r="AA172" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="173" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>93</v>
       </c>
@@ -9760,11 +9791,11 @@
       <c r="V173">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="W173" t="s">
+      <c r="AA173" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="174" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>94</v>
       </c>
@@ -9810,11 +9841,11 @@
       <c r="V174">
         <v>0.24110000000000001</v>
       </c>
-      <c r="W174" t="s">
+      <c r="AA174" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="175" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>94</v>
       </c>
@@ -9857,11 +9888,11 @@
       <c r="V175">
         <v>0.24110000000000001</v>
       </c>
-      <c r="W175" t="s">
+      <c r="AA175" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="176" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>94</v>
       </c>
@@ -9904,11 +9935,11 @@
       <c r="V176">
         <v>0.24110000000000001</v>
       </c>
-      <c r="W176" t="s">
+      <c r="AA176" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>94</v>
       </c>
@@ -9951,11 +9982,11 @@
       <c r="V177">
         <v>0.24110000000000001</v>
       </c>
-      <c r="W177" t="s">
+      <c r="AA177" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>94</v>
       </c>
@@ -9998,11 +10029,11 @@
       <c r="V178">
         <v>0.24110000000000001</v>
       </c>
-      <c r="W178" t="s">
+      <c r="AA178" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="179" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>94</v>
       </c>
@@ -10045,11 +10076,11 @@
       <c r="V179">
         <v>0.24110000000000001</v>
       </c>
-      <c r="W179" t="s">
+      <c r="AA179" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="180" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>94</v>
       </c>
@@ -10092,11 +10123,11 @@
       <c r="V180">
         <v>0.24110000000000001</v>
       </c>
-      <c r="W180" t="s">
+      <c r="AA180" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="181" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>95</v>
       </c>
@@ -10142,11 +10173,11 @@
       <c r="V181">
         <v>4.5100000000000001E-2</v>
       </c>
-      <c r="W181" t="s">
+      <c r="AA181" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>95</v>
       </c>
@@ -10195,11 +10226,11 @@
       <c r="V182">
         <v>4.5100000000000001E-2</v>
       </c>
-      <c r="W182" t="s">
+      <c r="AA182" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="183" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>95</v>
       </c>
@@ -10242,11 +10273,11 @@
       <c r="V183">
         <v>4.5100000000000001E-2</v>
       </c>
-      <c r="W183" t="s">
+      <c r="AA183" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>95</v>
       </c>
@@ -10289,11 +10320,11 @@
       <c r="V184">
         <v>4.5100000000000001E-2</v>
       </c>
-      <c r="W184" t="s">
+      <c r="AA184" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="185" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>95</v>
       </c>
@@ -10336,11 +10367,11 @@
       <c r="V185">
         <v>4.5100000000000001E-2</v>
       </c>
-      <c r="W185" t="s">
+      <c r="AA185" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>95</v>
       </c>
@@ -10383,11 +10414,11 @@
       <c r="V186">
         <v>4.5100000000000001E-2</v>
       </c>
-      <c r="W186" t="s">
+      <c r="AA186" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>96</v>
       </c>
@@ -10436,11 +10467,11 @@
       <c r="V187">
         <v>3.875E-2</v>
       </c>
-      <c r="W187" t="s">
+      <c r="AA187" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="188" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>96</v>
       </c>
@@ -10489,11 +10520,11 @@
       <c r="V188">
         <v>3.875E-2</v>
       </c>
-      <c r="W188" t="s">
+      <c r="AA188" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>96</v>
       </c>
@@ -10536,11 +10567,11 @@
       <c r="V189">
         <v>3.875E-2</v>
       </c>
-      <c r="W189" t="s">
+      <c r="AA189" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="190" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>96</v>
       </c>
@@ -10583,11 +10614,11 @@
       <c r="V190">
         <v>3.875E-2</v>
       </c>
-      <c r="W190" t="s">
+      <c r="AA190" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="191" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>96</v>
       </c>
@@ -10630,11 +10661,11 @@
       <c r="V191">
         <v>3.875E-2</v>
       </c>
-      <c r="W191" t="s">
+      <c r="AA191" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="192" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>96</v>
       </c>
@@ -10677,11 +10708,11 @@
       <c r="V192">
         <v>3.875E-2</v>
       </c>
-      <c r="W192" t="s">
+      <c r="AA192" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="193" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>99</v>
       </c>
@@ -10730,11 +10761,11 @@
       <c r="V193">
         <v>4.24E-2</v>
       </c>
-      <c r="W193" t="s">
+      <c r="AA193" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="194" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>99</v>
       </c>
@@ -10783,11 +10814,11 @@
       <c r="V194">
         <v>4.24E-2</v>
       </c>
-      <c r="W194" t="s">
+      <c r="AA194" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>99</v>
       </c>
@@ -10830,11 +10861,11 @@
       <c r="V195">
         <v>4.24E-2</v>
       </c>
-      <c r="W195" t="s">
+      <c r="AA195" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="196" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>99</v>
       </c>
@@ -10877,11 +10908,11 @@
       <c r="V196">
         <v>4.24E-2</v>
       </c>
-      <c r="W196" t="s">
+      <c r="AA196" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="197" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>99</v>
       </c>
@@ -10924,11 +10955,11 @@
       <c r="V197">
         <v>4.24E-2</v>
       </c>
-      <c r="W197" t="s">
+      <c r="AA197" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="198" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>99</v>
       </c>
@@ -10971,11 +11002,11 @@
       <c r="V198">
         <v>4.24E-2</v>
       </c>
-      <c r="W198" t="s">
+      <c r="AA198" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="199" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>100</v>
       </c>
@@ -11024,11 +11055,11 @@
       <c r="V199">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="W199" t="s">
+      <c r="AA199" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="200" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>100</v>
       </c>
@@ -11077,11 +11108,11 @@
       <c r="V200">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="W200" t="s">
+      <c r="AA200" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="201" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>100</v>
       </c>
@@ -11124,11 +11155,11 @@
       <c r="V201">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="W201" t="s">
+      <c r="AA201" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="202" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>100</v>
       </c>
@@ -11171,11 +11202,11 @@
       <c r="V202">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="W202" t="s">
+      <c r="AA202" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="203" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>100</v>
       </c>
@@ -11218,11 +11249,11 @@
       <c r="V203">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="W203" t="s">
+      <c r="AA203" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="204" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>100</v>
       </c>
@@ -11265,11 +11296,11 @@
       <c r="V204">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="W204" t="s">
+      <c r="AA204" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="205" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>101</v>
       </c>
@@ -11321,11 +11352,11 @@
       <c r="V205">
         <v>4.9599999999999998E-2</v>
       </c>
-      <c r="W205" t="s">
+      <c r="AA205" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="206" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>101</v>
       </c>
@@ -11380,11 +11411,11 @@
       <c r="V206">
         <v>4.9599999999999998E-2</v>
       </c>
-      <c r="W206" t="s">
+      <c r="AA206" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="207" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>101</v>
       </c>
@@ -11427,11 +11458,11 @@
       <c r="V207">
         <v>4.9599999999999998E-2</v>
       </c>
-      <c r="W207" t="s">
+      <c r="AA207" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="208" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>101</v>
       </c>
@@ -11474,11 +11505,11 @@
       <c r="V208">
         <v>4.9599999999999998E-2</v>
       </c>
-      <c r="W208" t="s">
+      <c r="AA208" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="209" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>101</v>
       </c>
@@ -11521,11 +11552,11 @@
       <c r="V209">
         <v>4.9599999999999998E-2</v>
       </c>
-      <c r="W209" t="s">
+      <c r="AA209" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="210" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>102</v>
       </c>
@@ -11574,11 +11605,11 @@
       <c r="V210">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="W210" t="s">
+      <c r="AA210" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="211" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>102</v>
       </c>
@@ -11627,11 +11658,11 @@
       <c r="V211">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="W211" t="s">
+      <c r="AA211" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="212" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>102</v>
       </c>
@@ -11671,11 +11702,11 @@
       <c r="V212">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="W212" t="s">
+      <c r="AA212" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="213" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>102</v>
       </c>
@@ -11718,11 +11749,11 @@
       <c r="V213">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="W213" t="s">
+      <c r="AA213" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="214" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>102</v>
       </c>
@@ -11765,11 +11796,11 @@
       <c r="V214">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="W214" t="s">
+      <c r="AA214" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="215" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>102</v>
       </c>
@@ -11812,11 +11843,11 @@
       <c r="V215">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="W215" t="s">
+      <c r="AA215" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="216" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>102</v>
       </c>
@@ -11862,11 +11893,11 @@
       <c r="V216">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="W216" t="s">
+      <c r="AA216" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="217" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>103</v>
       </c>
@@ -11915,11 +11946,11 @@
       <c r="V217">
         <v>0.10299999999999999</v>
       </c>
-      <c r="W217" t="s">
+      <c r="AA217" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="218" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>103</v>
       </c>
@@ -11968,11 +11999,11 @@
       <c r="V218">
         <v>0.10299999999999999</v>
       </c>
-      <c r="W218" t="s">
+      <c r="AA218" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="219" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>103</v>
       </c>
@@ -12015,11 +12046,11 @@
       <c r="V219">
         <v>0.10299999999999999</v>
       </c>
-      <c r="W219" t="s">
+      <c r="AA219" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="220" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>103</v>
       </c>
@@ -12062,11 +12093,11 @@
       <c r="V220">
         <v>0.10299999999999999</v>
       </c>
-      <c r="W220" t="s">
+      <c r="AA220" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="221" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>103</v>
       </c>
@@ -12109,11 +12140,11 @@
       <c r="V221">
         <v>0.10299999999999999</v>
       </c>
-      <c r="W221" t="s">
+      <c r="AA221" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="222" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>104</v>
       </c>
@@ -12156,11 +12187,11 @@
       <c r="V222">
         <v>0.10299999999999999</v>
       </c>
-      <c r="W222" t="s">
+      <c r="AA222" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="223" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>104</v>
       </c>
@@ -12209,11 +12240,11 @@
       <c r="V223">
         <v>0.15620000000000001</v>
       </c>
-      <c r="W223" t="s">
+      <c r="AA223" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="224" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>104</v>
       </c>
@@ -12262,11 +12293,11 @@
       <c r="V224">
         <v>0.15620000000000001</v>
       </c>
-      <c r="W224" t="s">
+      <c r="AA224" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="225" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>104</v>
       </c>
@@ -12309,11 +12340,11 @@
       <c r="V225">
         <v>0.15620000000000001</v>
       </c>
-      <c r="W225" t="s">
+      <c r="AA225" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="226" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>104</v>
       </c>
@@ -12356,11 +12387,11 @@
       <c r="V226">
         <v>0.15620000000000001</v>
       </c>
-      <c r="W226" t="s">
+      <c r="AA226" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="227" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>104</v>
       </c>
@@ -12403,11 +12434,11 @@
       <c r="V227">
         <v>0.15620000000000001</v>
       </c>
-      <c r="W227" t="s">
+      <c r="AA227" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="228" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>104</v>
       </c>
@@ -12450,11 +12481,11 @@
       <c r="V228">
         <v>0.15620000000000001</v>
       </c>
-      <c r="W228" t="s">
+      <c r="AA228" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="229" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>105</v>
       </c>
@@ -12503,11 +12534,11 @@
       <c r="V229">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W229" t="s">
+      <c r="AA229" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="230" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>105</v>
       </c>
@@ -12556,11 +12587,11 @@
       <c r="V230">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W230" t="s">
+      <c r="AA230" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="231" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>105</v>
       </c>
@@ -12603,11 +12634,11 @@
       <c r="V231">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W231" t="s">
+      <c r="AA231" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="232" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>105</v>
       </c>
@@ -12650,11 +12681,11 @@
       <c r="V232">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W232" t="s">
+      <c r="AA232" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="233" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>105</v>
       </c>
@@ -12697,11 +12728,11 @@
       <c r="V233">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W233" t="s">
+      <c r="AA233" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="234" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>105</v>
       </c>
@@ -12744,11 +12775,11 @@
       <c r="V234">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W234" t="s">
+      <c r="AA234" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="235" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>106</v>
       </c>
@@ -12797,11 +12828,11 @@
       <c r="V235">
         <v>3.95E-2</v>
       </c>
-      <c r="W235" t="s">
+      <c r="AA235" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="236" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>106</v>
       </c>
@@ -12850,11 +12881,11 @@
       <c r="V236">
         <v>3.95E-2</v>
       </c>
-      <c r="W236" t="s">
+      <c r="AA236" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="237" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>106</v>
       </c>
@@ -12900,11 +12931,11 @@
       <c r="V237">
         <v>3.95E-2</v>
       </c>
-      <c r="W237" t="s">
+      <c r="AA237" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="238" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>106</v>
       </c>
@@ -12953,11 +12984,11 @@
       <c r="V238">
         <v>3.95E-2</v>
       </c>
-      <c r="W238" t="s">
+      <c r="AA238" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="239" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>106</v>
       </c>
@@ -13000,11 +13031,11 @@
       <c r="V239">
         <v>3.95E-2</v>
       </c>
-      <c r="W239" t="s">
+      <c r="AA239" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="240" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>106</v>
       </c>
@@ -13047,11 +13078,11 @@
       <c r="V240">
         <v>3.95E-2</v>
       </c>
-      <c r="W240" t="s">
+      <c r="AA240" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="241" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>106</v>
       </c>
@@ -13094,11 +13125,11 @@
       <c r="V241">
         <v>3.95E-2</v>
       </c>
-      <c r="W241" t="s">
+      <c r="AA241" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="242" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>106</v>
       </c>
@@ -13141,11 +13172,11 @@
       <c r="V242">
         <v>3.95E-2</v>
       </c>
-      <c r="W242" t="s">
+      <c r="AA242" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="243" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>107</v>
       </c>
@@ -13191,11 +13222,11 @@
       <c r="V243">
         <v>0.1154</v>
       </c>
-      <c r="W243" t="s">
+      <c r="AA243" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="244" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>107</v>
       </c>
@@ -13244,11 +13275,11 @@
       <c r="V244">
         <v>0.1154</v>
       </c>
-      <c r="W244" t="s">
+      <c r="AA244" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="245" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>107</v>
       </c>
@@ -13291,11 +13322,11 @@
       <c r="V245">
         <v>0.1154</v>
       </c>
-      <c r="W245" t="s">
+      <c r="AA245" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="246" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>107</v>
       </c>
@@ -13338,11 +13369,11 @@
       <c r="V246">
         <v>0.1154</v>
       </c>
-      <c r="W246" t="s">
+      <c r="AA246" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="247" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>107</v>
       </c>
@@ -13385,11 +13416,11 @@
       <c r="V247">
         <v>0.1154</v>
       </c>
-      <c r="W247" t="s">
+      <c r="AA247" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="248" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>107</v>
       </c>
@@ -13432,11 +13463,11 @@
       <c r="V248">
         <v>0.1154</v>
       </c>
-      <c r="W248" t="s">
+      <c r="AA248" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="249" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>108</v>
       </c>
@@ -13482,11 +13513,11 @@
       <c r="V249">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W249" t="s">
+      <c r="AA249" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="250" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>108</v>
       </c>
@@ -13535,11 +13566,11 @@
       <c r="V250">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W250" t="s">
+      <c r="AA250" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="251" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>108</v>
       </c>
@@ -13582,11 +13613,11 @@
       <c r="V251">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W251" t="s">
+      <c r="AA251" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="252" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>108</v>
       </c>
@@ -13629,11 +13660,11 @@
       <c r="V252">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W252" t="s">
+      <c r="AA252" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="253" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>108</v>
       </c>
@@ -13676,11 +13707,11 @@
       <c r="V253">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W253" t="s">
+      <c r="AA253" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="254" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>108</v>
       </c>
@@ -13723,11 +13754,11 @@
       <c r="V254">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W254" t="s">
+      <c r="AA254" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="255" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>108</v>
       </c>
@@ -13770,11 +13801,11 @@
       <c r="V255">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W255" t="s">
+      <c r="AA255" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="256" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>108</v>
       </c>
@@ -13817,11 +13848,11 @@
       <c r="V256">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W256" t="s">
+      <c r="AA256" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="257" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>109</v>
       </c>
@@ -13864,11 +13895,11 @@
       <c r="V257">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="W257" t="s">
+      <c r="AA257" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="258" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>109</v>
       </c>
@@ -13914,11 +13945,11 @@
       <c r="V258">
         <v>0.17269999999999999</v>
       </c>
-      <c r="W258" t="s">
+      <c r="AA258" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="259" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>109</v>
       </c>
@@ -13967,11 +13998,11 @@
       <c r="V259">
         <v>0.17269999999999999</v>
       </c>
-      <c r="W259" t="s">
+      <c r="AA259" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="260" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>109</v>
       </c>
@@ -14014,11 +14045,11 @@
       <c r="V260">
         <v>0.17269999999999999</v>
       </c>
-      <c r="W260" t="s">
+      <c r="AA260" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="261" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>109</v>
       </c>
@@ -14061,11 +14092,11 @@
       <c r="V261">
         <v>0.17269999999999999</v>
       </c>
-      <c r="W261" t="s">
+      <c r="AA261" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="262" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>109</v>
       </c>
@@ -14108,11 +14139,11 @@
       <c r="V262">
         <v>0.17269999999999999</v>
       </c>
-      <c r="W262" t="s">
+      <c r="AA262" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="263" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>109</v>
       </c>
@@ -14155,11 +14186,11 @@
       <c r="V263">
         <v>0.17269999999999999</v>
       </c>
-      <c r="W263" t="s">
+      <c r="AA263" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="264" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>109</v>
       </c>
@@ -14202,11 +14233,11 @@
       <c r="V264">
         <v>0.17269999999999999</v>
       </c>
-      <c r="W264" t="s">
+      <c r="AA264" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="265" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>109</v>
       </c>
@@ -14249,11 +14280,11 @@
       <c r="V265">
         <v>0.17269999999999999</v>
       </c>
-      <c r="W265" t="s">
+      <c r="AA265" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="266" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>109</v>
       </c>
@@ -14296,11 +14327,11 @@
       <c r="V266">
         <v>0.17269999999999999</v>
       </c>
-      <c r="W266" t="s">
+      <c r="AA266" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="267" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>110</v>
       </c>
@@ -14346,11 +14377,11 @@
       <c r="V267">
         <v>5.8299999999999998E-2</v>
       </c>
-      <c r="W267" t="s">
+      <c r="AA267" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="268" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>110</v>
       </c>
@@ -14399,11 +14430,11 @@
       <c r="V268">
         <v>5.8299999999999998E-2</v>
       </c>
-      <c r="W268" t="s">
+      <c r="AA268" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="269" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>110</v>
       </c>
@@ -14449,11 +14480,11 @@
       <c r="V269">
         <v>5.8299999999999998E-2</v>
       </c>
-      <c r="W269" t="s">
+      <c r="AA269" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="270" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>110</v>
       </c>
@@ -14496,11 +14527,11 @@
       <c r="V270">
         <v>5.8299999999999998E-2</v>
       </c>
-      <c r="W270" t="s">
+      <c r="AA270" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="271" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>110</v>
       </c>
@@ -14543,11 +14574,11 @@
       <c r="V271">
         <v>5.8299999999999998E-2</v>
       </c>
-      <c r="W271" t="s">
+      <c r="AA271" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="272" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>111</v>
       </c>
@@ -14593,11 +14624,11 @@
       <c r="V272">
         <v>5.9200000000000003E-2</v>
       </c>
-      <c r="W272" t="s">
+      <c r="AA272" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="273" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>111</v>
       </c>
@@ -14646,11 +14677,11 @@
       <c r="V273">
         <v>5.9200000000000003E-2</v>
       </c>
-      <c r="W273" t="s">
+      <c r="AA273" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="274" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>111</v>
       </c>
@@ -14696,11 +14727,11 @@
       <c r="V274">
         <v>5.9200000000000003E-2</v>
       </c>
-      <c r="W274" t="s">
+      <c r="AA274" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="275" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>111</v>
       </c>
@@ -14743,11 +14774,11 @@
       <c r="V275">
         <v>5.9200000000000003E-2</v>
       </c>
-      <c r="W275" t="s">
+      <c r="AA275" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="276" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>111</v>
       </c>
@@ -14790,11 +14821,11 @@
       <c r="V276">
         <v>5.9200000000000003E-2</v>
       </c>
-      <c r="W276" t="s">
+      <c r="AA276" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="277" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>111</v>
       </c>
@@ -14837,11 +14868,11 @@
       <c r="V277">
         <v>5.9200000000000003E-2</v>
       </c>
-      <c r="W277" t="s">
+      <c r="AA277" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="278" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>111</v>
       </c>
@@ -14884,11 +14915,11 @@
       <c r="V278">
         <v>5.9200000000000003E-2</v>
       </c>
-      <c r="W278" t="s">
+      <c r="AA278" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="279" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>111</v>
       </c>
@@ -14931,11 +14962,11 @@
       <c r="V279">
         <v>5.9200000000000003E-2</v>
       </c>
-      <c r="W279" t="s">
+      <c r="AA279" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="280" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>111</v>
       </c>
@@ -14978,11 +15009,11 @@
       <c r="V280">
         <v>5.9200000000000003E-2</v>
       </c>
-      <c r="W280" t="s">
+      <c r="AA280" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="281" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>112</v>
       </c>
@@ -15028,11 +15059,11 @@
       <c r="V281">
         <v>5.3100000000000001E-2</v>
       </c>
-      <c r="W281" t="s">
+      <c r="AA281" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="282" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>112</v>
       </c>
@@ -15081,11 +15112,11 @@
       <c r="V282">
         <v>5.3100000000000001E-2</v>
       </c>
-      <c r="W282" t="s">
+      <c r="AA282" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="283" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>112</v>
       </c>
@@ -15131,11 +15162,11 @@
       <c r="V283">
         <v>5.3100000000000001E-2</v>
       </c>
-      <c r="W283" t="s">
+      <c r="AA283" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="284" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>112</v>
       </c>
@@ -15178,11 +15209,11 @@
       <c r="V284">
         <v>5.3100000000000001E-2</v>
       </c>
-      <c r="W284" t="s">
+      <c r="AA284" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="285" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>112</v>
       </c>
@@ -15225,11 +15256,11 @@
       <c r="V285">
         <v>5.3100000000000001E-2</v>
       </c>
-      <c r="W285" t="s">
+      <c r="AA285" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="286" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>112</v>
       </c>
@@ -15272,11 +15303,11 @@
       <c r="V286">
         <v>5.3100000000000001E-2</v>
       </c>
-      <c r="W286" t="s">
+      <c r="AA286" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="287" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>112</v>
       </c>
@@ -15319,11 +15350,11 @@
       <c r="V287">
         <v>5.3100000000000001E-2</v>
       </c>
-      <c r="W287" t="s">
+      <c r="AA287" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="288" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>112</v>
       </c>
@@ -15366,11 +15397,11 @@
       <c r="V288">
         <v>5.3100000000000001E-2</v>
       </c>
-      <c r="W288" t="s">
+      <c r="AA288" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="289" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>112</v>
       </c>
@@ -15413,8 +15444,16 @@
       <c r="V289">
         <v>5.3100000000000001E-2</v>
       </c>
-      <c r="W289" t="s">
+      <c r="AA289" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="290" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>118</v>
+      </c>
+      <c r="B290">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>